<commit_message>
Updated Traceability Matrix / Test Plan
- Finished Test Plan, with each thing to test and description being written
- Finished Asset Plan
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3cc90b10e39af9e0/SNHU/GAM305_DigitalGameDev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B837E066-F427-4FE5-90AB-C8339EF7F09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A58CF7A-4861-400C-AEAA-DCBDE0DD8676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36470" yWindow="-4220" windowWidth="34920" windowHeight="18110" activeTab="1" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="-36470" yWindow="-4220" windowWidth="34920" windowHeight="18110" firstSheet="1" activeTab="2" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
-    <sheet name="Assets List" sheetId="3" r:id="rId2"/>
-    <sheet name="Test Plan" sheetId="2" r:id="rId3"/>
+    <sheet name="Test Plan" sheetId="2" r:id="rId2"/>
+    <sheet name="Assets List" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="149">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -232,12 +232,168 @@
     <t>Emma</t>
   </si>
   <si>
+    <t>Test Plan</t>
+  </si>
+  <si>
+    <t>Test Feature</t>
+  </si>
+  <si>
+    <t>Description of Test</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>Runtime Errors</t>
+  </si>
+  <si>
+    <t>Updates/Error Resolution</t>
+  </si>
+  <si>
+    <t>Player Movement</t>
+  </si>
+  <si>
+    <t>Make sure player can move left, right, and jump and have camer in fixed side-scroller position.</t>
+  </si>
+  <si>
+    <t>Player Jumping</t>
+  </si>
+  <si>
+    <t>Player is able to jump with the SPACEBAR</t>
+  </si>
+  <si>
+    <t>When game starts, health bar is visible</t>
+  </si>
+  <si>
+    <t>Player should be able to see their healthbar at the corner of the screen with all icons full when the level loads.</t>
+  </si>
+  <si>
+    <t>Player is able to get Collectable, and collectable kitten disappears</t>
+  </si>
+  <si>
+    <t>Player can successfully interact with a collectable (kitten) by moving in its collision box. It will then promptly disappear, and will call the UI blueprint to update.</t>
+  </si>
+  <si>
+    <t>Collectable UI updates according to the amount of kittens collected</t>
+  </si>
+  <si>
+    <t>When the player collects a collectable kitten, the UI counter will increase by 1, and will update correctly.</t>
+  </si>
+  <si>
+    <t>Player triggers Enemy Customer AI</t>
+  </si>
+  <si>
+    <t>When the player is within the Enemy Customer's AI behavior range, the Enemy AI will change behavior accordingly</t>
+  </si>
+  <si>
+    <t>Player gets caught by Enemy Customer</t>
+  </si>
+  <si>
+    <t>When the player gets caught by the Enemy Customer, they will be unable to move for a certain period of time, lose one life, and then released.</t>
+  </si>
+  <si>
+    <t>Player triggers Enemy Worker AI</t>
+  </si>
+  <si>
+    <t>When the player is within the Enemy Worker's AI behavior range, the Enemy AI will change behavior accordingly</t>
+  </si>
+  <si>
+    <t>Player gets sprayed with water by Worker</t>
+  </si>
+  <si>
+    <t>When the Enemy Worker AI sprays with a spray bottle and the player is within the range of the water, the player will lose one life</t>
+  </si>
+  <si>
+    <t>Player gets bounced away when interacting with Yarn Ball by its left or right</t>
+  </si>
+  <si>
+    <t>When the player touches the Yarn Ball's collision and the Player is to the left or right of the Yarn Ball, the Player will briefly be pushed (or bounced) away by the Yarn Ball.</t>
+  </si>
+  <si>
+    <t>Player gets bounced upwards when interacting with the top of the Yarn Ball</t>
+  </si>
+  <si>
+    <t>When the player touches the Yarn Ball's collision and the Player is on top of the Yarn Ball, the Player will be bounced upwards by the Yarn Ball.</t>
+  </si>
+  <si>
+    <t>Player gets caught in Quicksand Litterbox Trap</t>
+  </si>
+  <si>
+    <t>When the player is within the quicksand of the Litter Box, the player will sink and respawn to the nearest spawn point or start goal.</t>
+  </si>
+  <si>
+    <t>Player's speed is slowed when in Hairball's collision</t>
+  </si>
+  <si>
+    <t>When the player is within the collision box of the hairball, the Player's speed will slow. When the player is outside of the collision, the Player's speed will return to normal.</t>
+  </si>
+  <si>
+    <t>Player is able to interact with Catnip</t>
+  </si>
+  <si>
+    <t>When the Player is within the Catnip's collision box, the Player gets distracted by the Catnip and the losing screen plays.</t>
+  </si>
+  <si>
+    <t>Player gets sent back to the start goal (or last checkpoint) after getting in contact with Catnip</t>
+  </si>
+  <si>
+    <t>When the losing screen is done playing after having played with catnip, the player is sent to the last checkpoint or goal</t>
+  </si>
+  <si>
+    <t>Player regains health by interacting with Milk pickup</t>
+  </si>
+  <si>
+    <t>When the Player touches a Milk Pickup's collision, the Player will regain some health</t>
+  </si>
+  <si>
+    <t>Milk pickup disappears when picked up by the Player</t>
+  </si>
+  <si>
+    <t>After the Player regains some health from a Milk Pickup, the Pickup will instantly disappear.</t>
+  </si>
+  <si>
+    <t>Player health bar updates after interacting with Milk pickup</t>
+  </si>
+  <si>
+    <t>After the Player regains some health from a Milk Pickup and the Pickup disappears, the Player UI updates health as well.</t>
+  </si>
+  <si>
+    <t>Player moves faster when interacting with Treat pickup</t>
+  </si>
+  <si>
+    <t>When the Player interacts with a Treat Pickup, the Player's speed increases</t>
+  </si>
+  <si>
+    <t>Treat pickup disappears when picked up by the Player</t>
+  </si>
+  <si>
+    <t>After the Player's speed increases by interacting with a Treat, the Treat will instantly disappear</t>
+  </si>
+  <si>
+    <t>Player returns to normal speed after consuming a treat</t>
+  </si>
+  <si>
+    <t>Player moves back to normal speed after a certain amount of time has passed since consuming a treat</t>
+  </si>
+  <si>
+    <t>Player is able to interact with Lure Pickup, and visual indicators appear where uncollected kittens are</t>
+  </si>
+  <si>
+    <t>When Player interacts with lure pickup, Player sees arrows around the window screen showing the direction of where uncollected kittens are briefly.</t>
+  </si>
+  <si>
+    <t>Lure pickup disappears when player interacts with it</t>
+  </si>
+  <si>
+    <t>After the Player triggers the Lure effects, the Lure Pickup disappears.</t>
+  </si>
+  <si>
     <t>Asset Name</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Progress</t>
   </si>
   <si>
@@ -329,135 +485,6 @@
   </si>
   <si>
     <t>Parallax Background Sprite</t>
-  </si>
-  <si>
-    <t>Test Plan</t>
-  </si>
-  <si>
-    <t>Test Feature</t>
-  </si>
-  <si>
-    <t>Description of Test</t>
-  </si>
-  <si>
-    <t>Pass/Fail</t>
-  </si>
-  <si>
-    <t>Bugs</t>
-  </si>
-  <si>
-    <t>Runtime Errors</t>
-  </si>
-  <si>
-    <t>Updates/Error Resolution</t>
-  </si>
-  <si>
-    <t>Player Movement</t>
-  </si>
-  <si>
-    <t>Make sure player can move left, right, and jump and have camer in fixed side-scroller position.</t>
-  </si>
-  <si>
-    <t>Player Jumping</t>
-  </si>
-  <si>
-    <t>Player is able to jump with the SPACEBAR</t>
-  </si>
-  <si>
-    <t>When game starts, health bar is visible</t>
-  </si>
-  <si>
-    <t>Player should be able to see their healthbar at the corner of the screen with all icons full when the level loads.</t>
-  </si>
-  <si>
-    <t>Player Getting Collectable, and collectable kitten disappears</t>
-  </si>
-  <si>
-    <t>Player can successfully interact with a collectable (kitten) by moving in its collision box. It will then promptly disappear, and will call the UI blueprint to update.</t>
-  </si>
-  <si>
-    <t>Collectable UI updates according to the amount of kittens collected</t>
-  </si>
-  <si>
-    <t>When the player collects a collectable kitten, the UI counter will increase by 1, and will update correctly.</t>
-  </si>
-  <si>
-    <t>Player triggers Enemy Customer AI</t>
-  </si>
-  <si>
-    <t>When the player is within the Enemy Customer's AI behavior range, the Enemy AI will change behavior accordingly</t>
-  </si>
-  <si>
-    <t>Player gets caught by Enemy Customer</t>
-  </si>
-  <si>
-    <t>When the player gets caught by the Enemy Customer, they will be unable to move for a certain period of time, lose one life, and then released.</t>
-  </si>
-  <si>
-    <t>Player triggers Enemy Worker AI</t>
-  </si>
-  <si>
-    <t>When the player is within the Enemy Worker's AI behavior range, the Enemy AI will change behavior accordingly</t>
-  </si>
-  <si>
-    <t>Player gets sprayed with water by Worker</t>
-  </si>
-  <si>
-    <t>When the Enemy Worker AI sprays with a spray bottle and the player is within the range of the water, the player will lose one life</t>
-  </si>
-  <si>
-    <t>Player gets bounced away when interacting with Yarn Ball by its left or right</t>
-  </si>
-  <si>
-    <t>Player gets bounced upwards when interacting with the top of the Yarn Ball</t>
-  </si>
-  <si>
-    <t>Player gets caught in Quicksand Litterbox Trap</t>
-  </si>
-  <si>
-    <t>When the player is within the quicksand of the Litter Box, the player will sink and respawn to the nearest spawn point or start goal.</t>
-  </si>
-  <si>
-    <t>Player's speed is slowed when in Hairball's collision</t>
-  </si>
-  <si>
-    <t>When the player is within the collision box of the hairball, the Player's speed will slow. When the player is outside of the collision, the Player's speed will return to normal.</t>
-  </si>
-  <si>
-    <t>Player is able to interact with Catnip</t>
-  </si>
-  <si>
-    <t>When the Player is within the Catnip's collision box, the Player gets distracted by the Catnip and the losing screen plays</t>
-  </si>
-  <si>
-    <t>Player gets sent back to the start goal (or last checkpoint) after getting in contact with Catnip</t>
-  </si>
-  <si>
-    <t>When the losing screen is done playing after having played with catnip, the player is sent to the last checkpoint or goal</t>
-  </si>
-  <si>
-    <t>Player regains health by interacting with Milk pickup</t>
-  </si>
-  <si>
-    <t>Milk pickup disappears when picked up by the Player</t>
-  </si>
-  <si>
-    <t>Player health bar updates after interacting with Milk pickup</t>
-  </si>
-  <si>
-    <t>Player moves faster when interacting with Treat pickup</t>
-  </si>
-  <si>
-    <t>Treat pickup disappears when picked up by the Player</t>
-  </si>
-  <si>
-    <t>Player moves back to normal speed after a certain amount of time has passed since consuming a treat</t>
-  </si>
-  <si>
-    <t>When Player interacts with lure pickup, Player sees arrows around the window screen showing the direction of where uncollected kittens are briefly.</t>
-  </si>
-  <si>
-    <t>Lure pickup disappears when player interacts with it</t>
   </si>
 </sst>
 </file>
@@ -755,7 +782,7 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -777,6 +804,90 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -786,9 +897,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -798,83 +906,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -888,9 +924,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF3CACE"/>
       <color rgb="FFAE2B00"/>
       <color rgb="FF8B1500"/>
-      <color rgb="FFF3CACE"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1203,515 +1239,586 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I2"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="40" style="16" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" style="16" customWidth="1"/>
-    <col min="5" max="8" width="23.42578125" style="16" customWidth="1"/>
-    <col min="9" max="9" width="60.85546875" style="16" customWidth="1"/>
-    <col min="10" max="12" width="23.42578125" style="16" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="24.5703125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="40" style="10" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="10" customWidth="1"/>
+    <col min="5" max="8" width="23.42578125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="60.85546875" style="10" customWidth="1"/>
+    <col min="10" max="12" width="23.42578125" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-    </row>
-    <row r="2" spans="1:9" s="23" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:9" ht="80.25" customHeight="1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:9" ht="26.25" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="30"/>
-    </row>
-    <row r="5" spans="1:9" s="33" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A5" s="31" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="32"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="45.6" customHeight="1">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="52.5" customHeight="1">
-      <c r="B7" s="35" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="52.5" customHeight="1">
-      <c r="B8" s="36" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="36"/>
-    </row>
-    <row r="9" spans="1:9" ht="50.45" customHeight="1"/>
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9" spans="1:9" ht="50.45" customHeight="1">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+    </row>
     <row r="10" spans="1:9" ht="50.1" customHeight="1">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="H10" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="37" t="s">
+      <c r="I10" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51" customHeight="1">
-      <c r="B11" s="36" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="H11" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="36" t="s">
+      <c r="I11" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="33.950000000000003" customHeight="1">
-      <c r="B12" s="36" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H12" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="36" t="s">
+      <c r="I12" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="54.95" customHeight="1"/>
+    <row r="13" spans="1:9" ht="54.95" customHeight="1">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+    </row>
     <row r="14" spans="1:9" ht="81.599999999999994" customHeight="1">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="36" t="s">
+      <c r="H14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="20" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="48.95" customHeight="1">
-      <c r="B15" s="36" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="20" t="s">
         <v>28</v>
       </c>
+      <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:9" ht="36.6" customHeight="1">
-      <c r="B16" s="36" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="F16" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="36" t="s">
+      <c r="H16" s="20" t="s">
         <v>28</v>
       </c>
+      <c r="I16" s="26"/>
     </row>
     <row r="17" spans="1:9" ht="50.1" customHeight="1">
-      <c r="B17" s="36" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="G17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="36" t="s">
+      <c r="H17" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="42" customHeight="1"/>
+      <c r="I17" s="26"/>
+    </row>
+    <row r="18" spans="1:9" ht="42" customHeight="1">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+    </row>
     <row r="19" spans="1:9" ht="42.95" customHeight="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="36" t="s">
+      <c r="F19" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="36" t="s">
+      <c r="H19" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="36" t="s">
+      <c r="I19" s="20" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="60.75">
-      <c r="B20" s="36" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="36" t="s">
+      <c r="E20" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="20" t="s">
         <v>28</v>
       </c>
+      <c r="I20" s="26"/>
     </row>
     <row r="21" spans="1:9" ht="81.599999999999994" customHeight="1">
-      <c r="B21" s="36" t="s">
+      <c r="A21" s="26"/>
+      <c r="B21" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="F21" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="20" t="s">
         <v>28</v>
       </c>
+      <c r="I21" s="26"/>
     </row>
     <row r="22" spans="1:9" ht="37.5" customHeight="1">
-      <c r="B22" s="36" t="s">
+      <c r="A22" s="26"/>
+      <c r="B22" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="F22" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="36" t="s">
+      <c r="G22" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="36" t="s">
+      <c r="H22" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="36" t="s">
+      <c r="I22" s="20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="18.600000000000001" customHeight="1"/>
-    <row r="25" spans="1:9" s="38" customFormat="1" ht="72.599999999999994" customHeight="1">
-      <c r="A25" s="38" t="s">
+    <row r="24" spans="1:9" ht="18.600000000000001" customHeight="1">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+    </row>
+    <row r="25" spans="1:9" s="22" customFormat="1" ht="72.599999999999994" customHeight="1">
+      <c r="A25" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="38" t="s">
+      <c r="F25" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="32.450000000000003" customHeight="1"/>
-    <row r="33" s="16" customFormat="1"/>
-    <row r="34" s="16" customFormat="1"/>
-    <row r="35" s="16" customFormat="1"/>
-    <row r="36" s="16" customFormat="1"/>
-    <row r="37" s="16" customFormat="1"/>
-    <row r="38" s="16" customFormat="1"/>
-    <row r="39" s="16" customFormat="1"/>
-    <row r="40" s="16" customFormat="1"/>
-    <row r="41" s="16" customFormat="1"/>
-    <row r="42" s="16" customFormat="1"/>
-    <row r="43" s="16" customFormat="1"/>
-    <row r="44" s="16" customFormat="1"/>
-    <row r="45" s="16" customFormat="1"/>
-    <row r="46" s="16" customFormat="1"/>
-    <row r="47" s="16" customFormat="1"/>
-    <row r="48" s="16" customFormat="1"/>
-    <row r="49" s="16" customFormat="1"/>
-    <row r="50" s="16" customFormat="1"/>
-    <row r="51" s="16" customFormat="1"/>
-    <row r="52" s="16" customFormat="1"/>
-    <row r="53" s="16" customFormat="1"/>
-    <row r="54" s="16" customFormat="1"/>
-    <row r="55" s="16" customFormat="1"/>
-    <row r="56" s="16" customFormat="1"/>
-    <row r="57" s="16" customFormat="1"/>
-    <row r="58" s="16" customFormat="1"/>
+      <c r="H25" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="32.450000000000003" customHeight="1">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+    </row>
+    <row r="33" s="10" customFormat="1"/>
+    <row r="34" s="10" customFormat="1"/>
+    <row r="35" s="10" customFormat="1"/>
+    <row r="36" s="10" customFormat="1"/>
+    <row r="37" s="10" customFormat="1"/>
+    <row r="38" s="10" customFormat="1"/>
+    <row r="39" s="10" customFormat="1"/>
+    <row r="40" s="10" customFormat="1"/>
+    <row r="41" s="10" customFormat="1"/>
+    <row r="42" s="10" customFormat="1"/>
+    <row r="43" s="10" customFormat="1"/>
+    <row r="44" s="10" customFormat="1"/>
+    <row r="45" s="10" customFormat="1"/>
+    <row r="46" s="10" customFormat="1"/>
+    <row r="47" s="10" customFormat="1"/>
+    <row r="48" s="10" customFormat="1"/>
+    <row r="49" s="10" customFormat="1"/>
+    <row r="50" s="10" customFormat="1"/>
+    <row r="51" s="10" customFormat="1"/>
+    <row r="52" s="10" customFormat="1"/>
+    <row r="53" s="10" customFormat="1"/>
+    <row r="54" s="10" customFormat="1"/>
+    <row r="55" s="10" customFormat="1"/>
+    <row r="56" s="10" customFormat="1"/>
+    <row r="57" s="10" customFormat="1"/>
+    <row r="58" s="10" customFormat="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:I2"/>
@@ -1728,17 +1835,464 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
+  <dimension ref="A1:G51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="37.5" customHeight="1">
+      <c r="A1" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="93.75" customHeight="1">
+      <c r="A4" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+    </row>
+    <row r="5" spans="1:7" ht="136.5" customHeight="1">
+      <c r="A5" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+    </row>
+    <row r="6" spans="1:7" ht="136.5" customHeight="1">
+      <c r="A6" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+    </row>
+    <row r="7" spans="1:7" ht="74.099999999999994" customHeight="1">
+      <c r="A7" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+    </row>
+    <row r="8" spans="1:7" ht="74.099999999999994" customHeight="1">
+      <c r="A8" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" ht="96" customHeight="1">
+      <c r="A9" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" ht="97.5" customHeight="1">
+      <c r="A10" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" ht="84.75" customHeight="1">
+      <c r="A11" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" ht="104.25" customHeight="1">
+      <c r="A12" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" ht="97.5" customHeight="1">
+      <c r="A13" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+    </row>
+    <row r="14" spans="1:7" ht="106.5" customHeight="1">
+      <c r="A14" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+    </row>
+    <row r="15" spans="1:7" ht="105.6" customHeight="1">
+      <c r="A15" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+    </row>
+    <row r="16" spans="1:7" ht="75.599999999999994" customHeight="1">
+      <c r="A16" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+    </row>
+    <row r="17" spans="1:6" ht="70.5" customHeight="1">
+      <c r="A17" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+    </row>
+    <row r="18" spans="1:6" ht="107.25" customHeight="1">
+      <c r="A18" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+    </row>
+    <row r="19" spans="1:6" ht="88.5" customHeight="1">
+      <c r="A19" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+    </row>
+    <row r="20" spans="1:6" ht="82.5" customHeight="1">
+      <c r="A20" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+    </row>
+    <row r="21" spans="1:6" ht="79.5" customHeight="1">
+      <c r="A21" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+    </row>
+    <row r="22" spans="1:6" ht="72.95" customHeight="1">
+      <c r="A22" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+    </row>
+    <row r="23" spans="1:6" ht="85.5" customHeight="1">
+      <c r="A23" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+    </row>
+    <row r="24" spans="1:6" ht="84" customHeight="1">
+      <c r="A24" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+    </row>
+    <row r="25" spans="1:6" ht="99.75" customHeight="1">
+      <c r="A25" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+    </row>
+    <row r="26" spans="1:6" ht="88.5" customHeight="1">
+      <c r="A26" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+    </row>
+    <row r="27" spans="1:6" ht="78.75" customHeight="1"/>
+    <row r="28" spans="1:6" ht="78" customHeight="1">
+      <c r="A28" s="5"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" ht="93" customHeight="1">
+      <c r="A29" s="5"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" ht="66.75" customHeight="1">
+      <c r="A30" s="5"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" ht="75" customHeight="1">
+      <c r="A31" s="5"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" ht="69.75" customHeight="1">
+      <c r="A32" s="5"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" ht="80.25" customHeight="1">
+      <c r="A33" s="5"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" ht="101.25" customHeight="1">
+      <c r="A34" s="5"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="5"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="5"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="5"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="5"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="5"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="5"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="5"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="5"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="5"/>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="5"/>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="5"/>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="5"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="5"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="5"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="5"/>
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="5"/>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="5"/>
+      <c r="F51" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{717C0889-0BE8-474F-8342-2D4D72B4FA3A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AA2BE-4F3F-4DB7-8D45-0977C97C1494}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="44" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
     <col min="5" max="9" width="17.140625" style="1" customWidth="1"/>
@@ -1746,238 +2300,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.5" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" ht="27.75" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:9" ht="73.5" customHeight="1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:9" ht="27.75" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="30"/>
-    </row>
-    <row r="5" spans="1:9" s="41" customFormat="1" ht="16.5">
-      <c r="A5" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="40"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" s="25" customFormat="1" ht="16.5">
+      <c r="A5" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>126</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30.75">
       <c r="A15" s="1" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30.75">
       <c r="A16" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30.75">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30.75">
       <c r="A17" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>135</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>140</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>141</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>142</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>143</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1994,440 +2546,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
-  <dimension ref="A1:G51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
-  <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="6" max="6" width="42.5703125" customWidth="1"/>
-    <col min="7" max="7" width="38.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A1" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="93.75" customHeight="1">
-      <c r="A4" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:7" ht="136.5" customHeight="1">
-      <c r="A5" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" ht="136.5" customHeight="1">
-      <c r="A6" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" ht="74.099999999999994" customHeight="1">
-      <c r="A7" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" ht="74.099999999999994" customHeight="1">
-      <c r="A8" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" ht="96" customHeight="1">
-      <c r="A9" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" ht="97.5" customHeight="1">
-      <c r="A10" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:7" ht="84.75" customHeight="1">
-      <c r="A11" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" ht="104.25" customHeight="1">
-      <c r="A12" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:7" ht="97.5" customHeight="1">
-      <c r="A13" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:7" ht="106.5" customHeight="1">
-      <c r="A14" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:7" ht="105.6" customHeight="1">
-      <c r="A15" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A16" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A17" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="1:6" ht="167.45" customHeight="1">
-      <c r="A18" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" spans="1:6" ht="88.5" customHeight="1">
-      <c r="A19" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="1:6" ht="82.5" customHeight="1">
-      <c r="A20" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-    </row>
-    <row r="21" spans="1:6" ht="79.5" customHeight="1">
-      <c r="A21" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="1:6" ht="72.95" customHeight="1">
-      <c r="A22" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-    </row>
-    <row r="23" spans="1:6" ht="85.5" customHeight="1">
-      <c r="A23" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-    </row>
-    <row r="24" spans="1:6" ht="84" customHeight="1">
-      <c r="A24" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-    </row>
-    <row r="25" spans="1:6" ht="99.75" customHeight="1">
-      <c r="A25" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="1:6" ht="88.5" customHeight="1">
-      <c r="A26" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-    </row>
-    <row r="27" spans="1:6" ht="78.75" customHeight="1"/>
-    <row r="28" spans="1:6" ht="78" customHeight="1">
-      <c r="A28" s="5"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" ht="93" customHeight="1">
-      <c r="A29" s="5"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" ht="66.75" customHeight="1">
-      <c r="A30" s="5"/>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" ht="75" customHeight="1">
-      <c r="A31" s="5"/>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" ht="69.75" customHeight="1">
-      <c r="A32" s="5"/>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" ht="80.25" customHeight="1">
-      <c r="A33" s="5"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" ht="101.25" customHeight="1">
-      <c r="A34" s="5"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="5"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="5"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="5"/>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="5"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="5"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="5"/>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="5"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="5"/>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="5"/>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="5"/>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="5"/>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="5"/>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="5"/>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="5"/>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="5"/>
-      <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="5"/>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="5"/>
-      <c r="F51" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:F2"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{717C0889-0BE8-474F-8342-2D4D72B4FA3A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f716dd8a-49a0-4c40-b209-038e1651b548" xsi:nil="true"/>
+    <Notes xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2688,19 +2816,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f716dd8a-49a0-4c40-b209-038e1651b548" xsi:nil="true"/>
-    <Notes xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2708,5 +2833,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}"/>
 </file>
</xml_diff>

<commit_message>
added models for cat condo, chair, stool and table. Updated tracabilityMatrix.
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3cc90b10e39af9e0/SNHU/GAM305_DigitalGameDev/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Documents\TeamRepo\GAM-305-Unreal-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A58CF7A-4861-400C-AEAA-DCBDE0DD8676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB28EAC-B443-48F5-8643-9231DA3DABA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36470" yWindow="-4220" windowWidth="34920" windowHeight="18110" firstSheet="1" activeTab="2" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="7080" yWindow="1485" windowWidth="18765" windowHeight="11835" firstSheet="1" activeTab="2" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="150">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -485,13 +485,16 @@
   </si>
   <si>
     <t>Parallax Background Sprite</t>
+  </si>
+  <si>
+    <t>Basic Model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -782,7 +785,7 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -855,24 +858,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -905,12 +911,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -941,9 +941,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -981,7 +981,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1087,7 +1087,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1229,7 +1229,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1243,7 +1243,7 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="10" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="10" customWidth="1"/>
@@ -1255,65 +1255,65 @@
     <col min="13" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-    </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
-    </row>
-    <row r="3" spans="1:9" ht="80.25" customHeight="1">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30"/>
+    </row>
+    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
-    </row>
-    <row r="4" spans="1:9" ht="26.25" customHeight="1">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="34"/>
+    </row>
+    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
-    </row>
-    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1">
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="37"/>
+    </row>
+    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="45.6" customHeight="1">
+    <row r="6" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
@@ -1369,8 +1369,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="52.5" customHeight="1">
-      <c r="A7" s="26"/>
+    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>23</v>
       </c>
@@ -1396,8 +1395,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="52.5" customHeight="1">
-      <c r="A8" s="26"/>
+    <row r="8" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>26</v>
       </c>
@@ -1419,18 +1417,8 @@
       </c>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="50.45" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-    </row>
-    <row r="10" spans="1:9" ht="50.1" customHeight="1">
+    <row r="9" spans="1:9" ht="50.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>29</v>
       </c>
@@ -1459,8 +1447,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="51" customHeight="1">
-      <c r="A11" s="26"/>
+    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
         <v>33</v>
       </c>
@@ -1486,8 +1473,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="33.950000000000003" customHeight="1">
-      <c r="A12" s="26"/>
+    <row r="12" spans="1:9" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
         <v>36</v>
       </c>
@@ -1513,18 +1499,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="54.95" customHeight="1">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-    </row>
-    <row r="14" spans="1:9" ht="81.599999999999994" customHeight="1">
+    <row r="13" spans="1:9" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>39</v>
       </c>
@@ -1553,8 +1529,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="48.95" customHeight="1">
-      <c r="A15" s="26"/>
+    <row r="15" spans="1:9" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="20" t="s">
         <v>43</v>
       </c>
@@ -1576,10 +1551,8 @@
       <c r="H15" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="26"/>
-    </row>
-    <row r="16" spans="1:9" ht="36.6" customHeight="1">
-      <c r="A16" s="26"/>
+    </row>
+    <row r="16" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="20" t="s">
         <v>45</v>
       </c>
@@ -1601,10 +1574,8 @@
       <c r="H16" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="26"/>
-    </row>
-    <row r="17" spans="1:9" ht="50.1" customHeight="1">
-      <c r="A17" s="26"/>
+    </row>
+    <row r="17" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
         <v>47</v>
       </c>
@@ -1626,20 +1597,9 @@
       <c r="H17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="26"/>
-    </row>
-    <row r="18" spans="1:9" ht="42" customHeight="1">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-    </row>
-    <row r="19" spans="1:9" ht="42.95" customHeight="1">
+    </row>
+    <row r="18" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:9" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>49</v>
       </c>
@@ -1668,8 +1628,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="60.75">
-      <c r="A20" s="26"/>
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
         <v>53</v>
       </c>
@@ -1691,10 +1650,8 @@
       <c r="H20" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="26"/>
-    </row>
-    <row r="21" spans="1:9" ht="81.599999999999994" customHeight="1">
-      <c r="A21" s="26"/>
+    </row>
+    <row r="21" spans="1:9" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>55</v>
       </c>
@@ -1716,10 +1673,8 @@
       <c r="H21" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="26"/>
-    </row>
-    <row r="22" spans="1:9" ht="37.5" customHeight="1">
-      <c r="A22" s="26"/>
+    </row>
+    <row r="22" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
         <v>57</v>
       </c>
@@ -1745,18 +1700,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="18.600000000000001" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-    </row>
-    <row r="25" spans="1:9" s="22" customFormat="1" ht="72.599999999999994" customHeight="1">
+    <row r="24" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:9" s="22" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>60</v>
       </c>
@@ -1782,43 +1727,33 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="32.450000000000003" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-    </row>
-    <row r="33" s="10" customFormat="1"/>
-    <row r="34" s="10" customFormat="1"/>
-    <row r="35" s="10" customFormat="1"/>
-    <row r="36" s="10" customFormat="1"/>
-    <row r="37" s="10" customFormat="1"/>
-    <row r="38" s="10" customFormat="1"/>
-    <row r="39" s="10" customFormat="1"/>
-    <row r="40" s="10" customFormat="1"/>
-    <row r="41" s="10" customFormat="1"/>
-    <row r="42" s="10" customFormat="1"/>
-    <row r="43" s="10" customFormat="1"/>
-    <row r="44" s="10" customFormat="1"/>
-    <row r="45" s="10" customFormat="1"/>
-    <row r="46" s="10" customFormat="1"/>
-    <row r="47" s="10" customFormat="1"/>
-    <row r="48" s="10" customFormat="1"/>
-    <row r="49" s="10" customFormat="1"/>
-    <row r="50" s="10" customFormat="1"/>
-    <row r="51" s="10" customFormat="1"/>
-    <row r="52" s="10" customFormat="1"/>
-    <row r="53" s="10" customFormat="1"/>
-    <row r="54" s="10" customFormat="1"/>
-    <row r="55" s="10" customFormat="1"/>
-    <row r="56" s="10" customFormat="1"/>
-    <row r="57" s="10" customFormat="1"/>
-    <row r="58" s="10" customFormat="1"/>
+    <row r="26" spans="1:9" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:I2"/>
@@ -1842,7 +1777,7 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" customWidth="1"/>
@@ -1853,29 +1788,29 @@
     <col min="7" max="7" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
-    </row>
-    <row r="2" spans="1:7" ht="37.5" customHeight="1">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="40"/>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>65</v>
       </c>
@@ -1896,376 +1831,376 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="93.75" customHeight="1">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-    </row>
-    <row r="5" spans="1:7" ht="136.5" customHeight="1">
-      <c r="A5" s="26" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-    </row>
-    <row r="6" spans="1:7" ht="136.5" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-    </row>
-    <row r="7" spans="1:7" ht="74.099999999999994" customHeight="1">
-      <c r="A7" s="26" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-    </row>
-    <row r="8" spans="1:7" ht="74.099999999999994" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-    </row>
-    <row r="9" spans="1:7" ht="96" customHeight="1">
-      <c r="A9" s="26" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-    </row>
-    <row r="10" spans="1:7" ht="97.5" customHeight="1">
-      <c r="A10" s="26" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-    </row>
-    <row r="11" spans="1:7" ht="84.75" customHeight="1">
-      <c r="A11" s="26" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-    </row>
-    <row r="12" spans="1:7" ht="104.25" customHeight="1">
-      <c r="A12" s="26" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-    </row>
-    <row r="13" spans="1:7" ht="97.5" customHeight="1">
-      <c r="A13" s="26" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-    </row>
-    <row r="14" spans="1:7" ht="106.5" customHeight="1">
-      <c r="A14" s="26" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-    </row>
-    <row r="15" spans="1:7" ht="105.6" customHeight="1">
-      <c r="A15" s="26" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-    </row>
-    <row r="16" spans="1:7" ht="75.599999999999994" customHeight="1">
-      <c r="A16" s="26" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-    </row>
-    <row r="17" spans="1:6" ht="70.5" customHeight="1">
-      <c r="A17" s="26" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-    </row>
-    <row r="18" spans="1:6" ht="107.25" customHeight="1">
-      <c r="A18" s="26" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-    </row>
-    <row r="19" spans="1:6" ht="88.5" customHeight="1">
-      <c r="A19" s="26" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-    </row>
-    <row r="20" spans="1:6" ht="82.5" customHeight="1">
-      <c r="A20" s="26" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-    </row>
-    <row r="21" spans="1:6" ht="79.5" customHeight="1">
-      <c r="A21" s="26" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-    </row>
-    <row r="22" spans="1:6" ht="72.95" customHeight="1">
-      <c r="A22" s="26" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-    </row>
-    <row r="23" spans="1:6" ht="85.5" customHeight="1">
-      <c r="A23" s="26" t="s">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-    </row>
-    <row r="24" spans="1:6" ht="84" customHeight="1">
-      <c r="A24" s="26" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-    </row>
-    <row r="25" spans="1:6" ht="99.75" customHeight="1">
-      <c r="A25" s="26" t="s">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-    </row>
-    <row r="26" spans="1:6" ht="88.5" customHeight="1">
-      <c r="A26" s="26" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-    </row>
-    <row r="27" spans="1:6" ht="78.75" customHeight="1"/>
-    <row r="28" spans="1:6" ht="78" customHeight="1">
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" ht="93" customHeight="1">
+    <row r="29" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" ht="66.75" customHeight="1">
+    <row r="30" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="75" customHeight="1">
+    <row r="31" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="69.75" customHeight="1">
+    <row r="32" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="80.25" customHeight="1">
+    <row r="33" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="101.25" customHeight="1">
+    <row r="34" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="F51" s="3"/>
     </row>
@@ -2285,83 +2220,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AA2BE-4F3F-4DB7-8D45-0977C97C1494}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="44" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="27" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
     <col min="5" max="9" width="17.140625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.5" customHeight="1">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-    </row>
-    <row r="2" spans="1:9" ht="27.75" customHeight="1">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+    </row>
+    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
-    </row>
-    <row r="3" spans="1:9" ht="73.5" customHeight="1">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30"/>
+    </row>
+    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
-    </row>
-    <row r="4" spans="1:9" ht="27.75" customHeight="1">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="34"/>
+    </row>
+    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
-    </row>
-    <row r="5" spans="1:9" s="25" customFormat="1" ht="16.5">
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="37"/>
+    </row>
+    <row r="5" spans="1:9" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="26" t="s">
         <v>118</v>
       </c>
       <c r="C5" s="23" t="s">
@@ -2374,160 +2309,160 @@
       <c r="H5" s="23"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="27" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30.75">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30.75">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30.75">
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="27" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B31" s="44" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="B31" s="27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="44" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="B32" s="27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B33" s="44" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="B33" s="27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="27" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>148</v>
       </c>
@@ -2825,13 +2760,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
+    <ds:schemaRef ds:uri="f716dd8a-49a0-4c40-b209-038e1651b548"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B87576-EBB2-43B7-B881-33A6175934F9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B87576-EBB2-43B7-B881-33A6175934F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
+    <ds:schemaRef ds:uri="f716dd8a-49a0-4c40-b209-038e1651b548"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
EndGoal logic and setup
Setup an actor blueprint for the EndGoal in a new folder under the 'Bri' folder called 'GameplayLogic'. EndGoal is nothing more than a box collision at the moment with an on event begin overlap that triggers when the player comes into contact with it and checks the amount of kitten collectibles held. If kittens is >= 10 then print string says "Success All kittens collected" if the kittens < 10 and player gets to the EndGoal then print string says "Failed to collect all 10 kittens". Updated traceability matrix.
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\BBanuelos_GAM305\TeamRepo\GAM-305-Unreal-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D3449E-02C1-4F1D-BB71-A68A5D01D465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41EE057-9EDB-4BC4-B318-BE1FA02415F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36470" yWindow="-4220" windowWidth="34920" windowHeight="18110" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="-36470" yWindow="-4220" windowWidth="34980" windowHeight="18110" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="165">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -485,6 +485,54 @@
   </si>
   <si>
     <t>Parallax Background Sprite</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Player start point</t>
+  </si>
+  <si>
+    <t>Player exit/end point</t>
+  </si>
+  <si>
+    <t>location for the start of the level</t>
+  </si>
+  <si>
+    <t>location where player ends/finishes the level</t>
+  </si>
+  <si>
+    <t>Gameplay/Meta</t>
+  </si>
+  <si>
+    <t>win condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">player must obtain 10 kitens (collectible pickups) throughout the level before reaching the end goal and without getting caught by enemies or side-tracked by obstacles </t>
+  </si>
+  <si>
+    <t>player makes it to end point without all the kittens, gets caught by enemies, and gets side-tracked by obstacle</t>
+  </si>
+  <si>
+    <t>Added win/lose condition logic for kittenCollectibles held by the player. If kittens &gt;= 10 then WIN, if kittens &lt; 10 then LOSE. No UI as of yet. Simple print strings for programming testing purposes.</t>
+  </si>
+  <si>
+    <t>lose condition (kittens &lt; 10)</t>
+  </si>
+  <si>
+    <t>lose condition (caught by customer)</t>
+  </si>
+  <si>
+    <t>Print string in place for verfication. UI to be added later.</t>
+  </si>
+  <si>
+    <t>lose condition (disciplined by café worker)</t>
+  </si>
+  <si>
+    <t>When player is caught by customer enemy, player loses, game is paused, and given option to restart level.</t>
+  </si>
+  <si>
+    <t>When player is caught by café worker enemy, player loses, game is paused, and given option to restart level.</t>
   </si>
 </sst>
 </file>
@@ -1236,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1725,22 +1773,159 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="34" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="35" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="36" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="37" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="38" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="39" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="40" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="41" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="42" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="43" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="44" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="45" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="46" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="47" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="48" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B28" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A30" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B31" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B32" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="49" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="50" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="51" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -2491,15 +2676,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003FC679AA94041F4BA4494D199A3447AF" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f196c085cfdbd30e0a6b7617037a918">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xmlns:ns3="f716dd8a-49a0-4c40-b209-038e1651b548" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c32ca31bb9a34b5b0e8feded347fb44b" ns2:_="" ns3:_="">
     <xsd:import namespace="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
@@ -2756,6 +2932,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
   <ds:schemaRefs>
@@ -2768,14 +2953,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B87576-EBB2-43B7-B881-33A6175934F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2792,4 +2969,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Obstacles setup 3 out of 4
The catnip, yarn ball, and hairball obstacles have been programmed.
Had to go into the BP_PaperPlayerChar blueprint a bit to tackle how to efficiently set the speed multipliers for the character concerning the hairball (slow movement speed) obstacle. This will come in handy for when I program the speed pickup later.

Planning to program the last obstacle when I tackle player health so I can see if the player is taking damage.
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\BBanuelos_GAM305\TeamRepo\GAM-305-Unreal-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41EE057-9EDB-4BC4-B318-BE1FA02415F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0E310A-EF56-4AA3-A527-148475C5EA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36470" yWindow="-4220" windowWidth="34980" windowHeight="18110" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="166">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Create a stationery object that upon player overlap will bounce the player backwards a certain distance.</t>
   </si>
   <si>
-    <t>May need to play with player and obstacle gravity depending on the effects of the bounce during testing.</t>
-  </si>
-  <si>
     <t>Quicksand Trap (Litter Box)</t>
   </si>
   <si>
@@ -214,12 +211,6 @@
     <t>Return to start (Catnip)</t>
   </si>
   <si>
-    <t>Create staionery object that upon overlap causes player to restart level.</t>
-  </si>
-  <si>
-    <t>Looks to be the easiest to accomplish for alpha testing purposes. Willing to help with any UI blueprint needs.</t>
-  </si>
-  <si>
     <t>UI</t>
   </si>
   <si>
@@ -533,6 +524,18 @@
   </si>
   <si>
     <t>When player is caught by café worker enemy, player loses, game is paused, and given option to restart level.</t>
+  </si>
+  <si>
+    <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected.</t>
+  </si>
+  <si>
+    <t>Create staionery object that upon overlap causes player to start of level.</t>
+  </si>
+  <si>
+    <t>Made using player's actor location and obstacle actor location, subtracting the values, then normalizing the result and multiplying that by a float variable called BounceStrength and adding that to a vector to give some upward movement from the bounce, and plugging all that into a Launch Character. The strength and distance can be adjusted using the BounceStrength variable and the Z value in the Make Vector node.</t>
+  </si>
+  <si>
+    <t>Made by adding new variable to BP_PaperPlayerChar called baseMoveSpeed and setting it on BeginPlay using get character movement -&gt; get max walk speed, then made a new function with the BP_PaperPlayerChar to set the speed multiplier to be called in the obstacle blueprint. In obstacle blueprint, on event begin overlap, casts to player calls SetSpeedMultiplier function and has '0.5' for the multipler before wiring to a set timer by event, that wires to a custom event called RestorePlayerSpeed that calls the SetSpeedMultiplier function where the multiplier is '1.0' for the event.  **Can be made into a Begin and End overlap obstacle instead of timer.</t>
   </si>
 </sst>
 </file>
@@ -1284,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1644,41 +1647,41 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:9" ht="43" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="20" t="s">
+    <row r="19" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="20" t="s">
+      <c r="E19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>52</v>
+      <c r="H19" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="B20" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>53</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>54</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>18</v>
@@ -1696,65 +1699,68 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="81.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="20" t="s">
+    <row r="21" spans="1:9" ht="151" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="D21" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="C22" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E22" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" s="20" t="s">
+      <c r="G22" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>59</v>
+      <c r="H22" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:9" s="22" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>18</v>
@@ -1766,7 +1772,7 @@
         <v>27</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H25" s="22" t="s">
         <v>28</v>
@@ -1775,13 +1781,13 @@
     <row r="26" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" s="19" t="s">
         <v>149</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>152</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>18</v>
@@ -1801,10 +1807,10 @@
     </row>
     <row r="28" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B28" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>18</v>
@@ -1822,18 +1828,18 @@
         <v>21</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>18</v>
@@ -1851,15 +1857,15 @@
         <v>21</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B31" s="19" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>18</v>
@@ -1877,15 +1883,15 @@
         <v>21</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B32" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="20" t="s">
         <v>160</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>163</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>18</v>
@@ -1905,10 +1911,10 @@
     </row>
     <row r="33" spans="2:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B33" s="20" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>18</v>
@@ -1972,7 +1978,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="38" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -1994,31 +2000,31 @@
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -2027,10 +2033,10 @@
     </row>
     <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -2039,10 +2045,10 @@
     </row>
     <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -2051,10 +2057,10 @@
     </row>
     <row r="7" spans="1:7" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -2063,10 +2069,10 @@
     </row>
     <row r="8" spans="1:7" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -2075,10 +2081,10 @@
     </row>
     <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -2087,10 +2093,10 @@
     </row>
     <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -2099,10 +2105,10 @@
     </row>
     <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -2111,10 +2117,10 @@
     </row>
     <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -2123,10 +2129,10 @@
     </row>
     <row r="13" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -2135,10 +2141,10 @@
     </row>
     <row r="14" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -2147,10 +2153,10 @@
     </row>
     <row r="15" spans="1:7" ht="105.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -2159,10 +2165,10 @@
     </row>
     <row r="16" spans="1:7" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -2171,10 +2177,10 @@
     </row>
     <row r="17" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -2183,10 +2189,10 @@
     </row>
     <row r="18" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -2195,10 +2201,10 @@
     </row>
     <row r="19" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -2207,10 +2213,10 @@
     </row>
     <row r="20" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -2219,10 +2225,10 @@
     </row>
     <row r="21" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -2231,10 +2237,10 @@
     </row>
     <row r="22" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -2243,10 +2249,10 @@
     </row>
     <row r="23" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -2255,10 +2261,10 @@
     </row>
     <row r="24" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -2267,10 +2273,10 @@
     </row>
     <row r="25" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -2279,10 +2285,10 @@
     </row>
     <row r="26" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -2476,13 +2482,13 @@
     </row>
     <row r="5" spans="1:9" s="25" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -2493,160 +2499,160 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2676,6 +2682,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003FC679AA94041F4BA4494D199A3447AF" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f196c085cfdbd30e0a6b7617037a918">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xmlns:ns3="f716dd8a-49a0-4c40-b209-038e1651b548" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c32ca31bb9a34b5b0e8feded347fb44b" ns2:_="" ns3:_="">
     <xsd:import namespace="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
@@ -2932,15 +2947,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
   <ds:schemaRefs>
@@ -2953,6 +2959,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B87576-EBB2-43B7-B881-33A6175934F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2969,12 +2983,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjusted Level design, added Pastry counter/register, cat bridges, shelf models"
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Documents\TeamRepo\GAM-305-Unreal-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB28EAC-B443-48F5-8643-9231DA3DABA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD60AD0F-ACEF-4624-9E27-87DDD6DD529B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="1485" windowWidth="18765" windowHeight="11835" firstSheet="1" activeTab="2" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="9555" yWindow="1665" windowWidth="18765" windowHeight="11835" firstSheet="1" activeTab="1" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="151">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -488,6 +488,9 @@
   </si>
   <si>
     <t>Basic Model</t>
+  </si>
+  <si>
+    <t>Basic Model(Attached^)</t>
   </si>
 </sst>
 </file>
@@ -1773,7 +1776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -2220,8 +2223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AA2BE-4F3F-4DB7-8D45-0977C97C1494}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2439,22 +2442,31 @@
         <v>143</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="B35" s="27" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="B36" s="27" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>146</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2494,6 +2506,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003FC679AA94041F4BA4494D199A3447AF" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f196c085cfdbd30e0a6b7617037a918">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xmlns:ns3="f716dd8a-49a0-4c40-b209-038e1651b548" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c32ca31bb9a34b5b0e8feded347fb44b" ns2:_="" ns3:_="">
     <xsd:import namespace="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
@@ -2750,15 +2771,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
   <ds:schemaRefs>
@@ -2771,6 +2783,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B87576-EBB2-43B7-B881-33A6175934F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2787,12 +2807,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated README and Traceability Matrix
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Documents\TeamRepo\GAM-305-Unreal-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spise\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD60AD0F-ACEF-4624-9E27-87DDD6DD529B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CBBB64-9D13-475A-8B4F-9185BC971E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="1665" windowWidth="18765" windowHeight="11835" firstSheet="1" activeTab="1" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="178">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -136,27 +136,18 @@
     <t>Set basic enemy idle movement behavior using splines.</t>
   </si>
   <si>
-    <t>Using splines to set basic range of the enemies so they can be easily placed in multiple locations throughout the level.</t>
-  </si>
-  <si>
     <t>Player detected</t>
   </si>
   <si>
     <t>Set movement behavior for when the player is detected within a certain range of the enemy.</t>
   </si>
   <si>
-    <t>Going to use a collision box for AI detection range for player overlap event.</t>
-  </si>
-  <si>
     <t>Player caught</t>
   </si>
   <si>
     <t>Set up basic end/exit game for when player is caught by enemy.</t>
   </si>
   <si>
-    <t>Going to use enemy capsule and player capsule collision overlap event to trigger exit.</t>
-  </si>
-  <si>
     <t>Pickups</t>
   </si>
   <si>
@@ -196,9 +187,6 @@
     <t>Create a stationery object that upon player overlap will bounce the player backwards a certain distance.</t>
   </si>
   <si>
-    <t>May need to play with player and obstacle gravity depending on the effects of the bounce during testing.</t>
-  </si>
-  <si>
     <t>Quicksand Trap (Litter Box)</t>
   </si>
   <si>
@@ -214,12 +202,6 @@
     <t>Return to start (Catnip)</t>
   </si>
   <si>
-    <t>Create staionery object that upon overlap causes player to restart level.</t>
-  </si>
-  <si>
-    <t>Looks to be the easiest to accomplish for alpha testing purposes. Willing to help with any UI blueprint needs.</t>
-  </si>
-  <si>
     <t>UI</t>
   </si>
   <si>
@@ -409,39 +391,12 @@
     <t>Player Jumping Animation</t>
   </si>
   <si>
-    <t>Player Hurt Animation</t>
-  </si>
-  <si>
-    <t>Player Death Animation</t>
-  </si>
-  <si>
-    <t>Kitten Sprites (Uncollected)</t>
-  </si>
-  <si>
-    <t>Kitten Sprites (Collected)</t>
-  </si>
-  <si>
-    <t>Concept Art WIP</t>
-  </si>
-  <si>
     <t>Enemy Customer Roaming Sprite</t>
   </si>
   <si>
-    <t>Enemy Customer Following Sprite</t>
-  </si>
-  <si>
-    <t>Enemy Customer Grabbing Sprite</t>
-  </si>
-  <si>
     <t>Enemy Worker Roaming Sprite</t>
   </si>
   <si>
-    <t>Enemy Worker Following Sprite</t>
-  </si>
-  <si>
-    <t>Enemy Worker Spraying Sprite</t>
-  </si>
-  <si>
     <t>Yarn Ball Sprite</t>
   </si>
   <si>
@@ -487,17 +442,147 @@
     <t>Parallax Background Sprite</t>
   </si>
   <si>
-    <t>Basic Model</t>
-  </si>
-  <si>
-    <t>Basic Model(Attached^)</t>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Player start point</t>
+  </si>
+  <si>
+    <t>Player exit/end point</t>
+  </si>
+  <si>
+    <t>location for the start of the level</t>
+  </si>
+  <si>
+    <t>location where player ends/finishes the level</t>
+  </si>
+  <si>
+    <t>Gameplay/Meta</t>
+  </si>
+  <si>
+    <t>win condition</t>
+  </si>
+  <si>
+    <t>lose condition (caught by customer)</t>
+  </si>
+  <si>
+    <t>lose condition (disciplined by café worker)</t>
+  </si>
+  <si>
+    <t>When player is caught by customer enemy, player loses, game is paused, and given option to restart level.</t>
+  </si>
+  <si>
+    <t>When player is caught by café worker enemy, player loses, game is paused, and given option to restart level.</t>
+  </si>
+  <si>
+    <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected.</t>
+  </si>
+  <si>
+    <t>Create staionery object that upon overlap causes player to start of level.</t>
+  </si>
+  <si>
+    <t>Made using player's actor location and obstacle actor location, subtracting the values, then normalizing the result and multiplying that by a float variable called BounceStrength and adding that to a vector to give some upward movement from the bounce, and plugging all that into a Launch Character. The strength and distance can be adjusted using the BounceStrength variable and the Z value in the Make Vector node.</t>
+  </si>
+  <si>
+    <t>Made by adding new variable to BP_PaperPlayerChar called baseMoveSpeed and setting it on BeginPlay using get character movement -&gt; get max walk speed, then made a new function with the BP_PaperPlayerChar to set the speed multiplier to be called in the obstacle blueprint. In obstacle blueprint, on event begin overlap, casts to player calls SetSpeedMultiplier function and has '0.5' for the multipler before wiring to a set timer by event, that wires to a custom event called RestorePlayerSpeed that calls the SetSpeedMultiplier function where the multiplier is '1.0' for the event.  **Can be made into a Begin and End overlap obstacle instead of timer.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>UI not implemented yet, currently using PrintString</t>
+  </si>
+  <si>
+    <t>Currently set as timer function for slowed movement speed period, will adjust to an on begin and end overlap.</t>
+  </si>
+  <si>
+    <t>Currently set as a teleport back to start without losing items, can adjust cause player to lose game with a pause game and add UI for chance to restart</t>
+  </si>
+  <si>
+    <t>May need adjusted after playtest in level build to account appropriate jump height for platforms</t>
+  </si>
+  <si>
+    <t>Shelf</t>
+  </si>
+  <si>
+    <t>Concept Art Finished.</t>
+  </si>
+  <si>
+    <t>Kitten Sprites</t>
+  </si>
+  <si>
+    <t>Player Touches Catnip Sprite</t>
+  </si>
+  <si>
+    <t>Player Grabbed By Customer Sprite</t>
+  </si>
+  <si>
+    <t>Concept Art Finished. 
+Basic Models Completed.</t>
+  </si>
+  <si>
+    <t>Concept Art Finished.
+Basic Models Completed.</t>
+  </si>
+  <si>
+    <t>Concept Art Finished.
+Sprite Finished.</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Not Implemented.</t>
+  </si>
+  <si>
+    <t>May need to adjust bounce strength and z vector if bounce is too strong or too weak
+UPDATE: Bounce Strength has been updated, and is now a lot less frustrating!</t>
+  </si>
+  <si>
+    <t>Enemy Cat Toy</t>
+  </si>
+  <si>
+    <t>Enemy Customer collision has trouble collecting kitten. We are going to pivot directions and cut this enemy in the game in favor of one that will appear on the platforms instead in the Beta Release.</t>
+  </si>
+  <si>
+    <t>Enemy Cat Toy Patrols Around Specified Start and End Points</t>
+  </si>
+  <si>
+    <t>The Enemy Cat Toy will patrol on platforms to and from designated points (or coordinates) indefinitely.</t>
+  </si>
+  <si>
+    <t>Player gets hurt by Enemy Cat Toy</t>
+  </si>
+  <si>
+    <t>When the player collides with the Enemy Cat Toy, the player will take damage.</t>
+  </si>
+  <si>
+    <t>Enemies can move around randomly.</t>
+  </si>
+  <si>
+    <t>When the player is within the enemies' collisions, the enemies move towards the player.</t>
+  </si>
+  <si>
+    <t>The enemies currently do not do anything to the player other than follow them. While we can implement projectiles shooting at the player with the Enemy Worker AI, we will have to change the Enemy Customer AI to something more feasible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">player must obtain 10 kittens (collectible pickups) throughout the level before reaching the end goal and without getting caught by enemies or side-tracked by obstacles </t>
+  </si>
+  <si>
+    <t>Print string in place for verification. UI to be added later.</t>
+  </si>
+  <si>
+    <t>Added win condition logic for kittenCollectibles held by the player. If kittens &gt;= 10 then WIN. No UI as of yet. Simple print strings for programming testing purposes.</t>
+  </si>
+  <si>
+    <t>Enemy Customer will be replaced in favor of Enemy Cat Toy for Beta Release.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -616,8 +701,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -660,6 +752,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF3CACE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -788,7 +892,7 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -846,9 +950,6 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -867,6 +968,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -915,6 +1019,36 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1240,25 +1374,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="24.53125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="23.46484375" style="10" customWidth="1"/>
     <col min="3" max="3" width="40" style="10" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" style="10" customWidth="1"/>
-    <col min="5" max="8" width="23.42578125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="60.85546875" style="10" customWidth="1"/>
-    <col min="10" max="12" width="23.42578125" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="10"/>
+    <col min="4" max="4" width="25.53125" style="10" customWidth="1"/>
+    <col min="5" max="8" width="23.46484375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="60.796875" style="10" customWidth="1"/>
+    <col min="10" max="12" width="23.46484375" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="8.796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -1271,7 +1405,7 @@
       <c r="H1" s="32"/>
       <c r="I1" s="32"/>
     </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -1286,7 +1420,7 @@
       <c r="H2" s="29"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
@@ -1301,7 +1435,7 @@
       <c r="H3" s="33"/>
       <c r="I3" s="34"/>
     </row>
-    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
@@ -1316,7 +1450,7 @@
       <c r="H4" s="36"/>
       <c r="I4" s="37"/>
     </row>
-    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
@@ -1343,7 +1477,7 @@
       </c>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
@@ -1372,7 +1506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="19" t="s">
         <v>23</v>
       </c>
@@ -1398,7 +1532,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="20" t="s">
         <v>26</v>
       </c>
@@ -1420,68 +1554,69 @@
       </c>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="50.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+    <row r="9" spans="1:9" ht="50.55" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="1:9" s="53" customFormat="1" ht="50.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="21" t="s">
+      <c r="G10" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="52" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="53" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="54"/>
+      <c r="B11" s="51" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
+      <c r="C11" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="D11" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="51" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="20" t="s">
+      <c r="C12" s="20" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>37</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>18</v>
@@ -1493,51 +1628,51 @@
         <v>19</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="H12" s="20" t="s">
         <v>28</v>
       </c>
       <c r="I12" s="20" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="55.05" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="1:9" ht="81.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:9" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="D14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="20" t="s">
+    </row>
+    <row r="15" spans="1:9" ht="49.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C15" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>44</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>18</v>
@@ -1555,12 +1690,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="36.700000000000003" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>18</v>
@@ -1578,12 +1713,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="50.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>18</v>
@@ -1601,42 +1736,42 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:9" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+    <row r="18" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B20" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="C20" s="20" t="s">
         <v>50</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>54</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>18</v>
@@ -1654,109 +1789,213 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+    <row r="21" spans="1:9" ht="151.05000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="64.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C25" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D25" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E25" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="G25" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B28" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+      <c r="A30" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B31" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="F31" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="H31" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="20" t="s">
+    <row r="32" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B32" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="20" t="s">
+      <c r="E32" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="F32" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H32" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:9" s="22" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:I2"/>
@@ -1774,26 +2013,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.46484375" customWidth="1"/>
+    <col min="2" max="2" width="35.53125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="6" max="6" width="42.5703125" customWidth="1"/>
-    <col min="7" max="7" width="38.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.46484375" customWidth="1"/>
+    <col min="6" max="6" width="42.53125" customWidth="1"/>
+    <col min="7" max="7" width="38.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="38" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -1801,7 +2040,7 @@
       <c r="E1" s="39"/>
       <c r="F1" s="40"/>
     </row>
-    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -1813,399 +2052,489 @@
       <c r="E2" s="42"/>
       <c r="F2" s="43"/>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B4" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C4" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="B5" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="C5" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="B6" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:7" ht="74.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="74.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="55" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+    </row>
+    <row r="10" spans="1:7" s="45" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B10" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="C10" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="49" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+    </row>
+    <row r="12" spans="1:7" s="49" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+    </row>
+    <row r="13" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B13" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="10"/>
+        <v>82</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="105.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="10"/>
+        <v>88</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
     </row>
-    <row r="18" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="75.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="10"/>
+        <v>96</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C22" s="10"/>
+        <v>98</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="10" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C23" s="10"/>
+        <v>100</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="73.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="10" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C24" s="10"/>
+        <v>102</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="10" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C25" s="10"/>
+        <v>104</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C26" s="10"/>
+        <v>106</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="5"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="5"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="5"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="5"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="5"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="5"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="5"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="5"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="5"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="5"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="5"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="5"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="5"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="5"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="5"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="5"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="5"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="5"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="5"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="5"/>
       <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="5"/>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" s="5"/>
+      <c r="F53" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2221,23 +2550,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AA2BE-4F3F-4DB7-8D45-0977C97C1494}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="27" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.86328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.3984375" style="26" customWidth="1"/>
+    <col min="3" max="3" width="28.46484375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="9" width="17.140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="9" width="17.19921875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -2250,7 +2579,7 @@
       <c r="H1" s="32"/>
       <c r="I1" s="32"/>
     </row>
-    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -2265,7 +2594,7 @@
       <c r="H2" s="29"/>
       <c r="I2" s="30"/>
     </row>
-    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
@@ -2280,7 +2609,7 @@
       <c r="H3" s="33"/>
       <c r="I3" s="34"/>
     </row>
-    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
@@ -2295,188 +2624,210 @@
       <c r="H4" s="36"/>
       <c r="I4" s="37"/>
     </row>
-    <row r="5" spans="1:9" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:9" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="23"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="46" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A14" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B14" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="B15" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" s="27"/>
+    </row>
+    <row r="18" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B18" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B19" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B20" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B22" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B23" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B24" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B26" s="27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B27" s="27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B28" s="27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B29" s="27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B30" s="27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B31" s="27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B32" s="27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B32" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B34" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2506,15 +2857,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003FC679AA94041F4BA4494D199A3447AF" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f196c085cfdbd30e0a6b7617037a918">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xmlns:ns3="f716dd8a-49a0-4c40-b209-038e1651b548" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c32ca31bb9a34b5b0e8feded347fb44b" ns2:_="" ns3:_="">
     <xsd:import namespace="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
@@ -2771,6 +3113,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
   <ds:schemaRefs>
@@ -2783,14 +3134,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B87576-EBB2-43B7-B881-33A6175934F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2807,4 +3150,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated the Traceability Matrix and TestPlan
Updated matrix and test plan to current build and development progress and known bugs. Please make sure to pull from the repo again before you update it on your local machines and let others know when you update it. Sadly it is not like an Unreal project where our individual changes can be tracked and saved easily. We'll need to let each other know when we have it open and are making changes and pull after someone has pushed those changes before making our own to avoid overwriting each others changes.
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Documents\TeamRepo\GAM-305-Unreal-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\BBanuelos_GAM305\TeamRepo\GAM-305-Unreal-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD60AD0F-ACEF-4624-9E27-87DDD6DD529B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{82D5FF91-B755-4CC2-983C-F2D7C359B6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="1665" windowWidth="18765" windowHeight="11835" firstSheet="1" activeTab="1" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="-37100" yWindow="-4190" windowWidth="34980" windowHeight="18110" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="192">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -136,27 +136,18 @@
     <t>Set basic enemy idle movement behavior using splines.</t>
   </si>
   <si>
-    <t>Using splines to set basic range of the enemies so they can be easily placed in multiple locations throughout the level.</t>
-  </si>
-  <si>
     <t>Player detected</t>
   </si>
   <si>
     <t>Set movement behavior for when the player is detected within a certain range of the enemy.</t>
   </si>
   <si>
-    <t>Going to use a collision box for AI detection range for player overlap event.</t>
-  </si>
-  <si>
     <t>Player caught</t>
   </si>
   <si>
     <t>Set up basic end/exit game for when player is caught by enemy.</t>
   </si>
   <si>
-    <t>Going to use enemy capsule and player capsule collision overlap event to trigger exit.</t>
-  </si>
-  <si>
     <t>Pickups</t>
   </si>
   <si>
@@ -196,9 +187,6 @@
     <t>Create a stationery object that upon player overlap will bounce the player backwards a certain distance.</t>
   </si>
   <si>
-    <t>May need to play with player and obstacle gravity depending on the effects of the bounce during testing.</t>
-  </si>
-  <si>
     <t>Quicksand Trap (Litter Box)</t>
   </si>
   <si>
@@ -214,12 +202,6 @@
     <t>Return to start (Catnip)</t>
   </si>
   <si>
-    <t>Create staionery object that upon overlap causes player to restart level.</t>
-  </si>
-  <si>
-    <t>Looks to be the easiest to accomplish for alpha testing purposes. Willing to help with any UI blueprint needs.</t>
-  </si>
-  <si>
     <t>UI</t>
   </si>
   <si>
@@ -487,10 +469,151 @@
     <t>Parallax Background Sprite</t>
   </si>
   <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Player start point</t>
+  </si>
+  <si>
+    <t>Player exit/end point</t>
+  </si>
+  <si>
+    <t>location for the start of the level</t>
+  </si>
+  <si>
+    <t>location where player ends/finishes the level</t>
+  </si>
+  <si>
+    <t>Gameplay/Meta</t>
+  </si>
+  <si>
+    <t>win condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">player must obtain 10 kitens (collectible pickups) throughout the level before reaching the end goal and without getting caught by enemies or side-tracked by obstacles </t>
+  </si>
+  <si>
+    <t>player makes it to end point without all the kittens, gets caught by enemies, and gets side-tracked by obstacle</t>
+  </si>
+  <si>
+    <t>Added win/lose condition logic for kittenCollectibles held by the player. If kittens &gt;= 10 then WIN, if kittens &lt; 10 then LOSE. No UI as of yet. Simple print strings for programming testing purposes.</t>
+  </si>
+  <si>
+    <t>lose condition (kittens &lt; 10)</t>
+  </si>
+  <si>
+    <t>lose condition (caught by customer)</t>
+  </si>
+  <si>
+    <t>Print string in place for verfication. UI to be added later.</t>
+  </si>
+  <si>
+    <t>lose condition (disciplined by café worker)</t>
+  </si>
+  <si>
+    <t>When player is caught by customer enemy, player loses, game is paused, and given option to restart level.</t>
+  </si>
+  <si>
+    <t>When player is caught by café worker enemy, player loses, game is paused, and given option to restart level.</t>
+  </si>
+  <si>
+    <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected.</t>
+  </si>
+  <si>
+    <t>Create staionery object that upon overlap causes player to start of level.</t>
+  </si>
+  <si>
+    <t>Made using player's actor location and obstacle actor location, subtracting the values, then normalizing the result and multiplying that by a float variable called BounceStrength and adding that to a vector to give some upward movement from the bounce, and plugging all that into a Launch Character. The strength and distance can be adjusted using the BounceStrength variable and the Z value in the Make Vector node.</t>
+  </si>
+  <si>
+    <t>Made by adding new variable to BP_PaperPlayerChar called baseMoveSpeed and setting it on BeginPlay using get character movement -&gt; get max walk speed, then made a new function with the BP_PaperPlayerChar to set the speed multiplier to be called in the obstacle blueprint. In obstacle blueprint, on event begin overlap, casts to player calls SetSpeedMultiplier function and has '0.5' for the multipler before wiring to a set timer by event, that wires to a custom event called RestorePlayerSpeed that calls the SetSpeedMultiplier function where the multiplier is '1.0' for the event.  **Can be made into a Begin and End overlap obstacle instead of timer.</t>
+  </si>
+  <si>
+    <t>Moved from Bri to Emma</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>UI not implemented yet, currently using PrintString</t>
+  </si>
+  <si>
+    <t>May need to adjust bounce strength and z vector if bounce is too strong or too weak</t>
+  </si>
+  <si>
+    <t>Currently set as timer function for slowed movement speed period, will adjust to an on begin and end overlap.</t>
+  </si>
+  <si>
+    <t>Currently set as a teleport back to start without losing items, can adjust cause player to lose game with a pause game and add UI for chance to restart</t>
+  </si>
+  <si>
+    <t>May need adjusted after playtest in level build to account appropriate jump height for platforms</t>
+  </si>
+  <si>
     <t>Basic Model</t>
   </si>
   <si>
     <t>Basic Model(Attached^)</t>
+  </si>
+  <si>
+    <t>Y/N</t>
+  </si>
+  <si>
+    <t>Spawn point/checkpoint</t>
+  </si>
+  <si>
+    <t>a place for the player to return to that is not the start after they run into catnip after reaching a certain part of the level</t>
+  </si>
+  <si>
+    <t>Player HUD (Kittern Callectible) UI</t>
+  </si>
+  <si>
+    <t>UI to show how many kittens player has collected in the level</t>
+  </si>
+  <si>
+    <t>Game End (Success)</t>
+  </si>
+  <si>
+    <t>UI to display a successful win and if player would like to quit or play the game again</t>
+  </si>
+  <si>
+    <t>Game End (Failure)</t>
+  </si>
+  <si>
+    <t>UI to display a failure to complete level without getting caught and asking player if they would like to quit or restart level</t>
+  </si>
+  <si>
+    <t>Enemy follows but can't get close enough to player to trigger overlap event</t>
+  </si>
+  <si>
+    <t>Will need to change to a different kind of enemy type that will be on platforms to avoid the collision problem with environment objects.</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Need to update enemy logic/programming to shoot projectiles (water) at the player</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added a box collision actor blueprint to behind the player start so the player can't run off into the abyss at the beginning </t>
+  </si>
+  <si>
+    <t>Textures</t>
+  </si>
+  <si>
+    <t>Textures need to be added to the environment and platform objects</t>
+  </si>
+  <si>
+    <t>Alexis</t>
+  </si>
+  <si>
+    <t>Placeholder textures have been added for the alpha</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>Need background added to the level map</t>
   </si>
 </sst>
 </file>
@@ -788,7 +911,7 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -846,9 +969,6 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -914,6 +1034,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1240,83 +1367,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" style="10" customWidth="1"/>
     <col min="3" max="3" width="40" style="10" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" style="10" customWidth="1"/>
-    <col min="5" max="8" width="23.42578125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="60.85546875" style="10" customWidth="1"/>
-    <col min="10" max="12" width="23.42578125" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="10"/>
+    <col min="4" max="4" width="25.54296875" style="10" customWidth="1"/>
+    <col min="5" max="8" width="23.453125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="60.81640625" style="10" customWidth="1"/>
+    <col min="10" max="12" width="23.453125" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
-    </row>
-    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-    </row>
-    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37"/>
-    </row>
-    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
@@ -1343,7 +1470,7 @@
       </c>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="45.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
@@ -1372,7 +1499,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="19" t="s">
         <v>23</v>
       </c>
@@ -1398,7 +1525,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="20" t="s">
         <v>26</v>
       </c>
@@ -1420,147 +1547,134 @@
       </c>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="50.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+    <row r="9" spans="1:9" ht="50.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="43" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:9" ht="81.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:9" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="H15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="20" t="s">
+    </row>
+    <row r="16" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C16" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>46</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>18</v>
@@ -1577,13 +1691,14 @@
       <c r="H16" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>18</v>
@@ -1600,66 +1715,68 @@
       <c r="H17" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:9" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="B21" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="C21" s="20" t="s">
         <v>50</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>56</v>
       </c>
       <c r="D21" s="20" t="s">
         <v>18</v>
@@ -1676,87 +1793,374 @@
       <c r="H21" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
+      <c r="I21" s="20"/>
+    </row>
+    <row r="22" spans="1:9" ht="151" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="20" t="s">
+      <c r="H26" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D27" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E27" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F31" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="F33" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H33" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:9" s="22" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="22" t="s">
+      <c r="I33" s="44"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B34" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="44"/>
+    </row>
+    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B35" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E35" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F35" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="22" t="s">
+      <c r="G35" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="I35" s="45" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A37" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B38" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B39" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B40" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:I2"/>
@@ -1776,434 +2180,480 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="6" max="6" width="42.5703125" customWidth="1"/>
-    <col min="7" max="7" width="38.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.453125" customWidth="1"/>
+    <col min="6" max="6" width="42.54296875" customWidth="1"/>
+    <col min="7" max="7" width="38.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="40"/>
-    </row>
-    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B4" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C4" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="B5" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="C5" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="B6" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:7" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B10" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="C10" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B11" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="C11" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="105.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
     </row>
-    <row r="20" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="F51" s="3"/>
     </row>
@@ -2223,260 +2673,260 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AA2BE-4F3F-4DB7-8D45-0977C97C1494}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="27" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7265625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="9" width="17.140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="9" width="17.1796875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
-    </row>
-    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-    </row>
-    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37"/>
-    </row>
-    <row r="5" spans="1:9" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" s="24" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="23"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="26" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="23" t="s">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B13" s="26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B13" s="27" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B24" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B31" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B32" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B33" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B34" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="B35" s="26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B36" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B31" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B37" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B34" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2494,18 +2944,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f716dd8a-49a0-4c40-b209-038e1651b548" xsi:nil="true"/>
-    <Notes xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2514,7 +2952,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003FC679AA94041F4BA4494D199A3447AF" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f196c085cfdbd30e0a6b7617037a918">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xmlns:ns3="f716dd8a-49a0-4c40-b209-038e1651b548" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c32ca31bb9a34b5b0e8feded347fb44b" ns2:_="" ns3:_="">
     <xsd:import namespace="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
@@ -2771,18 +3209,19 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
-    <ds:schemaRef ds:uri="f716dd8a-49a0-4c40-b209-038e1651b548"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f716dd8a-49a0-4c40-b209-038e1651b548" xsi:nil="true"/>
+    <Notes xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2790,7 +3229,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B87576-EBB2-43B7-B881-33A6175934F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2807,4 +3246,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
+    <ds:schemaRef ds:uri="f716dd8a-49a0-4c40-b209-038e1651b548"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating matrix and test plan
Uploading updated matrix and test plan to main repo with all the progress that has been made to reflect the same as what is on the Final Alpha branch.
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spise\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\BBanuelos_GAM305\TeamRepo\GAM-305-Unreal-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2C046F-66BF-482B-B95B-E3F4676C6773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{82D5FF91-B755-4CC2-983C-F2D7C359B6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="10943" windowHeight="12863" activeTab="1" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="-37100" yWindow="-4190" windowWidth="34980" windowHeight="18110" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="192">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -391,12 +391,39 @@
     <t>Player Jumping Animation</t>
   </si>
   <si>
+    <t>Player Hurt Animation</t>
+  </si>
+  <si>
+    <t>Player Death Animation</t>
+  </si>
+  <si>
+    <t>Kitten Sprites (Uncollected)</t>
+  </si>
+  <si>
+    <t>Kitten Sprites (Collected)</t>
+  </si>
+  <si>
+    <t>Concept Art WIP</t>
+  </si>
+  <si>
     <t>Enemy Customer Roaming Sprite</t>
   </si>
   <si>
+    <t>Enemy Customer Following Sprite</t>
+  </si>
+  <si>
+    <t>Enemy Customer Grabbing Sprite</t>
+  </si>
+  <si>
     <t>Enemy Worker Roaming Sprite</t>
   </si>
   <si>
+    <t>Enemy Worker Following Sprite</t>
+  </si>
+  <si>
+    <t>Enemy Worker Spraying Sprite</t>
+  </si>
+  <si>
     <t>Yarn Ball Sprite</t>
   </si>
   <si>
@@ -523,31 +550,70 @@
     <t>May need adjusted after playtest in level build to account appropriate jump height for platforms</t>
   </si>
   <si>
-    <t>Shelf</t>
-  </si>
-  <si>
-    <t>Concept Art Finished.</t>
-  </si>
-  <si>
-    <t>Kitten Sprites</t>
-  </si>
-  <si>
-    <t>Player Touches Catnip Sprite</t>
-  </si>
-  <si>
-    <t>Player Grabbed By Customer Sprite</t>
-  </si>
-  <si>
-    <t>Concept Art Finished. 
-Basic Models Completed.</t>
-  </si>
-  <si>
-    <t>Concept Art Finished.
-Basic Models Completed.</t>
-  </si>
-  <si>
-    <t>Concept Art Finished.
-Sprite Finished.</t>
+    <t>Basic Model</t>
+  </si>
+  <si>
+    <t>Basic Model(Attached^)</t>
+  </si>
+  <si>
+    <t>Y/N</t>
+  </si>
+  <si>
+    <t>Spawn point/checkpoint</t>
+  </si>
+  <si>
+    <t>a place for the player to return to that is not the start after they run into catnip after reaching a certain part of the level</t>
+  </si>
+  <si>
+    <t>Player HUD (Kittern Callectible) UI</t>
+  </si>
+  <si>
+    <t>UI to show how many kittens player has collected in the level</t>
+  </si>
+  <si>
+    <t>Game End (Success)</t>
+  </si>
+  <si>
+    <t>UI to display a successful win and if player would like to quit or play the game again</t>
+  </si>
+  <si>
+    <t>Game End (Failure)</t>
+  </si>
+  <si>
+    <t>UI to display a failure to complete level without getting caught and asking player if they would like to quit or restart level</t>
+  </si>
+  <si>
+    <t>Enemy follows but can't get close enough to player to trigger overlap event</t>
+  </si>
+  <si>
+    <t>Will need to change to a different kind of enemy type that will be on platforms to avoid the collision problem with environment objects.</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Need to update enemy logic/programming to shoot projectiles (water) at the player</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added a box collision actor blueprint to behind the player start so the player can't run off into the abyss at the beginning </t>
+  </si>
+  <si>
+    <t>Textures</t>
+  </si>
+  <si>
+    <t>Textures need to be added to the environment and platform objects</t>
+  </si>
+  <si>
+    <t>Alexis</t>
+  </si>
+  <si>
+    <t>Placeholder textures have been added for the alpha</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>Need background added to the level map</t>
   </si>
 </sst>
 </file>
@@ -845,7 +911,7 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -903,9 +969,6 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -972,8 +1035,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1300,83 +1367,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.53125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="23.46484375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" style="10" customWidth="1"/>
     <col min="3" max="3" width="40" style="10" customWidth="1"/>
-    <col min="4" max="4" width="25.53125" style="10" customWidth="1"/>
-    <col min="5" max="8" width="23.46484375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="60.796875" style="10" customWidth="1"/>
-    <col min="10" max="12" width="23.46484375" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="8.796875" style="10"/>
+    <col min="4" max="4" width="25.54296875" style="10" customWidth="1"/>
+    <col min="5" max="8" width="23.453125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="60.81640625" style="10" customWidth="1"/>
+    <col min="10" max="12" width="23.453125" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
-    </row>
-    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-    </row>
-    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37"/>
-    </row>
-    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
@@ -1403,7 +1470,7 @@
       </c>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="45.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
@@ -1432,7 +1499,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="19" t="s">
         <v>23</v>
       </c>
@@ -1458,7 +1525,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="20" t="s">
         <v>26</v>
       </c>
@@ -1480,147 +1547,134 @@
       </c>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="50.55" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="10" spans="1:9" ht="50.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="20" t="s">
+    <row r="9" spans="1:9" ht="50.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="20" t="s">
+      <c r="H10" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="43" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="20" t="s">
+      <c r="H11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="55.05" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="14" spans="1:9" ht="81.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="18" t="s">
+      <c r="H12" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:9" ht="81.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C15" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I15" s="19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="49.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="20" t="s">
+    <row r="16" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C16" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="36.700000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>43</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>18</v>
@@ -1637,13 +1691,14 @@
       <c r="H16" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="50.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>18</v>
@@ -1660,92 +1715,92 @@
       <c r="H17" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="19" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="18" t="s">
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B20" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C20" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D20" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E20" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F20" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G20" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H20" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B20" s="20" t="s">
+      <c r="I20" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="B21" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C21" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D21" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E21" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F21" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G21" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H21" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="151.05000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="19" t="s">
+      <c r="I21" s="20"/>
+    </row>
+    <row r="22" spans="1:9" ht="151" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C22" s="19" t="s">
         <v>52</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="64.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>151</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>18</v>
@@ -1754,7 +1809,7 @@
         <v>19</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>20</v>
@@ -1763,124 +1818,132 @@
         <v>21</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="18.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="25" spans="1:9" s="22" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B26" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C26" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D26" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E26" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F26" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G26" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H26" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D27" s="19" t="s">
+    <row r="27" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D27" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B28" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="D28" s="19" t="s">
+      <c r="E27" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28" s="19" t="s">
+      <c r="E28" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="18" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="57" x14ac:dyDescent="0.45">
-      <c r="A30" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30" s="19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B31" s="19" t="s">
         <v>144</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>18</v>
@@ -1898,38 +1961,41 @@
         <v>21</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B32" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="D32" s="20" t="s">
+      <c r="C32" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G32" s="20" t="s">
+      <c r="E32" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H32" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="H32" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B33" s="20" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>18</v>
@@ -1946,17 +2012,155 @@
       <c r="H33" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="49" s="10" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="50" s="10" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="51" s="10" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="52" s="10" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="53" s="10" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="54" s="10" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="55" s="10" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="56" s="10" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="57" s="10" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="58" s="10" customFormat="1" x14ac:dyDescent="0.45"/>
+      <c r="I33" s="44"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B34" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="44"/>
+    </row>
+    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B35" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="I35" s="45" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A37" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B38" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B39" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B40" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:I2"/>
@@ -1976,44 +2180,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.46484375" customWidth="1"/>
-    <col min="2" max="2" width="35.53125" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="35.46484375" customWidth="1"/>
-    <col min="6" max="6" width="42.53125" customWidth="1"/>
-    <col min="7" max="7" width="38.796875" customWidth="1"/>
+    <col min="5" max="5" width="35.453125" customWidth="1"/>
+    <col min="6" max="6" width="42.54296875" customWidth="1"/>
+    <col min="7" max="7" width="38.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="40"/>
-    </row>
-    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>59</v>
       </c>
@@ -2034,7 +2238,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>65</v>
       </c>
@@ -2042,13 +2246,13 @@
         <v>66</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>67</v>
       </c>
@@ -2056,15 +2260,15 @@
         <v>68</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>69</v>
       </c>
@@ -2076,7 +2280,7 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="74.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>71</v>
       </c>
@@ -2089,10 +2293,10 @@
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
       <c r="F7" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="74.2" customHeight="1" x14ac:dyDescent="0.45">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>73</v>
       </c>
@@ -2105,46 +2309,62 @@
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="s">
+      <c r="C9" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="10" t="s">
+      <c r="C10" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>81</v>
       </c>
@@ -2156,7 +2376,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
         <v>83</v>
       </c>
@@ -2164,15 +2384,15 @@
         <v>84</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
         <v>85</v>
       </c>
@@ -2180,15 +2400,15 @@
         <v>86</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="105.7" customHeight="1" x14ac:dyDescent="0.45">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="105.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>87</v>
       </c>
@@ -2200,7 +2420,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="75.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>89</v>
       </c>
@@ -2213,10 +2433,10 @@
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>91</v>
       </c>
@@ -2229,10 +2449,10 @@
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>93</v>
       </c>
@@ -2244,7 +2464,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>95</v>
       </c>
@@ -2256,7 +2476,7 @@
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
     </row>
-    <row r="20" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>97</v>
       </c>
@@ -2268,7 +2488,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>99</v>
       </c>
@@ -2280,7 +2500,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" ht="73.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>101</v>
       </c>
@@ -2292,7 +2512,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>103</v>
       </c>
@@ -2304,7 +2524,7 @@
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>105</v>
       </c>
@@ -2316,7 +2536,7 @@
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>107</v>
       </c>
@@ -2328,7 +2548,7 @@
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>109</v>
       </c>
@@ -2340,100 +2560,100 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="F51" s="3"/>
     </row>
@@ -2451,275 +2671,262 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AA2BE-4F3F-4DB7-8D45-0977C97C1494}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.86328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.3984375" style="27" customWidth="1"/>
-    <col min="3" max="3" width="28.46484375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7265625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="9" width="17.19921875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.19921875" style="1"/>
+    <col min="5" max="9" width="17.1796875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
-    </row>
-    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-    </row>
-    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37"/>
-    </row>
-    <row r="5" spans="1:9" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="23" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+    </row>
+    <row r="5" spans="1:9" s="24" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="23"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="44" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="44" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="B19" s="44" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B26" s="44" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B27" s="44" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="44" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B29" s="44" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B30" s="44" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="44" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+        <v>134</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B32" s="44" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+        <v>137</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Player Any Damage Health Pickup
Adjusted player blueprint by adding an EventAnyDamage that uses float variables health, maxHealth, newHealth for logic and quits game if player's health reaches 0.

Added player Health Pickup that adds health but does not exceed player's maxHealth variable. Disappears upon overlap and adds to health without going over maxHealth.

Created 2 different litter obstacles. 1 is a damage causer using apply damage node, I used to verify the player takes damage and can gain health via health pickup. The other is a true quicksand trap that has a 2 second delay while sinking before respawning back to start.
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\BBanuelos_GAM305\TeamRepo\GAM-305-Unreal-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82D5FF91-B755-4CC2-983C-F2D7C359B6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE73853-873A-4FFE-88DE-6E3F93B2B506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37100" yWindow="-4190" windowWidth="34980" windowHeight="18110" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="-37100" yWindow="-4190" windowWidth="34980" windowHeight="18110" activeTab="1" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="200">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -517,9 +517,6 @@
     <t>When player is caught by café worker enemy, player loses, game is paused, and given option to restart level.</t>
   </si>
   <si>
-    <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected.</t>
-  </si>
-  <si>
     <t>Create staionery object that upon overlap causes player to start of level.</t>
   </si>
   <si>
@@ -541,9 +538,6 @@
     <t>May need to adjust bounce strength and z vector if bounce is too strong or too weak</t>
   </si>
   <si>
-    <t>Currently set as timer function for slowed movement speed period, will adjust to an on begin and end overlap.</t>
-  </si>
-  <si>
     <t>Currently set as a teleport back to start without losing items, can adjust cause player to lose game with a pause game and add UI for chance to restart</t>
   </si>
   <si>
@@ -614,6 +608,36 @@
   </si>
   <si>
     <t>Need background added to the level map</t>
+  </si>
+  <si>
+    <t>Currently goes back to start point. Will setup respawn point actor blueprint soon.</t>
+  </si>
+  <si>
+    <t>Hairball movement was adjusted to a begin and end overlap for slowing player down.</t>
+  </si>
+  <si>
+    <t>Player takes damage on EventAnyDamage using float variables health, newHealth, and maxHealth, where health - damage clamped (0-maxHealth) sets health which sets newHealth, where if newHealth is &lt;= 0 then the game quits, if the player still has health a print string shows the players remaining health upon damage.</t>
+  </si>
+  <si>
+    <t>DamageTrap (Litter Box)</t>
+  </si>
+  <si>
+    <t>Created by casting to player and using apply damage node.</t>
+  </si>
+  <si>
+    <t>Create stationery object that when player comes into contact with will be unable to jkump and will sink into until reset back to start or spawn point</t>
+  </si>
+  <si>
+    <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected. ***Need to do respawn point logic</t>
+  </si>
+  <si>
+    <t>Has a begin and end overlap event incase player is able to escape. Set gravity to zero and pull character through the floor using velocity and setting new bool variable added to player called canJump? that gets set to false upon overlap with a current delay of 2 seconds before respawning back to start. ***Need to do respawn point logic</t>
+  </si>
+  <si>
+    <t>Currentlt have set to restore health by 10 with the health clamped between 0-maxHealth (which is set to 100). Adds 10 health on overlap only if player has less than maxHealth. Disappears upon overlap regardless if pllayer is at full health or not.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currently set to send back to start. Will setup respawn actor blueprint soon. </t>
   </si>
 </sst>
 </file>
@@ -987,60 +1011,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1367,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1386,62 +1410,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
     </row>
     <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="36"/>
     </row>
     <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
@@ -1525,27 +1549,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="20" t="s">
+    <row r="8" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="20"/>
+      <c r="H8" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="50.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1573,8 +1599,8 @@
       <c r="H10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="43" t="s">
-        <v>163</v>
+      <c r="I10" s="27" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
@@ -1600,7 +1626,7 @@
         <v>21</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
@@ -1623,10 +1649,10 @@
         <v>57</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
@@ -1669,29 +1695,31 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="20" t="s">
+    <row r="16" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="20"/>
+      <c r="H16" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="20" t="s">
@@ -1768,48 +1796,51 @@
         <v>21</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="B21" s="20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21"/>
+      <c r="B21" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="B22" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="20"/>
-    </row>
-    <row r="22" spans="1:9" ht="151" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>52</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>20</v>
@@ -1818,15 +1849,15 @@
         <v>21</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="151" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>160</v>
+        <v>52</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>18</v>
@@ -1835,7 +1866,7 @@
         <v>19</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>20</v>
@@ -1844,62 +1875,68 @@
         <v>21</v>
       </c>
       <c r="I23" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="21" t="s">
+      <c r="D24" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B27" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C27" s="21" t="s">
         <v>56</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="H26" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>176</v>
       </c>
       <c r="D27" s="21" t="s">
         <v>18</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>27</v>
       </c>
+      <c r="G27" s="21" t="s">
+        <v>57</v>
+      </c>
       <c r="H27" s="21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="21" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D28" s="21" t="s">
         <v>18</v>
@@ -1916,10 +1953,10 @@
     </row>
     <row r="29" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="21" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D29" s="21" t="s">
         <v>18</v>
@@ -1934,42 +1971,36 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="18" t="s">
+    <row r="30" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B32" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C32" s="19" t="s">
         <v>146</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I31" s="19" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>147</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>18</v>
@@ -1987,114 +2018,114 @@
         <v>21</v>
       </c>
       <c r="I32" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="19" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B33" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="D33" s="20" t="s">
+    <row r="34" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B34" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I33" s="44"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B34" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="D34" s="20"/>
       <c r="E34" s="20" t="s">
         <v>27</v>
       </c>
       <c r="F34" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G34" s="20"/>
+      <c r="G34" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="H34" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I34" s="44"/>
-    </row>
-    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="B35" s="18" t="s">
+      <c r="I34" s="28"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B35" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="28"/>
+    </row>
+    <row r="36" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B36" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="H36" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="I36" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="D35" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="I35" s="45" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A37" s="18" t="s">
+    </row>
+    <row r="38" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A38" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B38" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C38" s="19" t="s">
         <v>150</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H37" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I37" s="19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B38" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>151</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>18</v>
@@ -2116,34 +2147,37 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B39" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="D39" s="20" t="s">
+      <c r="B39" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G39" s="20" t="s">
+      <c r="E39" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H39" s="20" t="s">
-        <v>28</v>
+      <c r="H39" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" s="19" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B40" s="20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>18</v>
@@ -2158,6 +2192,29 @@
         <v>20</v>
       </c>
       <c r="H40" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B41" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" s="20" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2180,8 +2237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2196,26 +2253,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="45"/>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
@@ -2246,7 +2303,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -2260,12 +2317,12 @@
         <v>68</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2293,7 +2350,7 @@
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
       <c r="F7" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -2309,7 +2366,7 @@
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.35">
@@ -2323,11 +2380,11 @@
         <v>61</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2338,14 +2395,14 @@
         <v>78</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2356,12 +2413,12 @@
         <v>80</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
       <c r="F11" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2384,12 +2441,12 @@
         <v>84</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2400,40 +2457,44 @@
         <v>86</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="105.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="C15" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18" t="s">
-        <v>167</v>
+      <c r="C16" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2449,44 +2510,52 @@
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="C18" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="C19" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="C20" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
@@ -2688,62 +2757,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
     </row>
     <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="36"/>
     </row>
     <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:9" s="24" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -2868,7 +2937,7 @@
         <v>134</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -2876,7 +2945,7 @@
         <v>135</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -2884,7 +2953,7 @@
         <v>136</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -2892,7 +2961,7 @@
         <v>137</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -2900,7 +2969,7 @@
         <v>138</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -2908,7 +2977,7 @@
         <v>139</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -2916,7 +2985,7 @@
         <v>140</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -2953,6 +3022,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f716dd8a-49a0-4c40-b209-038e1651b548" xsi:nil="true"/>
+    <Notes xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003FC679AA94041F4BA4494D199A3447AF" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f196c085cfdbd30e0a6b7617037a918">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xmlns:ns3="f716dd8a-49a0-4c40-b209-038e1651b548" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c32ca31bb9a34b5b0e8feded347fb44b" ns2:_="" ns3:_="">
     <xsd:import namespace="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
@@ -3209,18 +3290,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f716dd8a-49a0-4c40-b209-038e1651b548" xsi:nil="true"/>
-    <Notes xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
   <ds:schemaRefs>
@@ -3230,6 +3299,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
+    <ds:schemaRef ds:uri="f716dd8a-49a0-4c40-b209-038e1651b548"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B87576-EBB2-43B7-B881-33A6175934F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3246,15 +3326,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
-    <ds:schemaRef ds:uri="f716dd8a-49a0-4c40-b209-038e1651b548"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Merge pull request #15 from nmalma/beta-release"
This reverts commit f794cadf8b44761361864ffa72123b1d5d65fd25, reversing
changes made to d104214c4f66a03d02a6e3f99a1d82a97d4f78c6.
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\BBanuelos_GAM305\TeamRepo\GAM-305-Unreal-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F89C95EB-D896-4C79-AE5C-3960334D77D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{82D5FF91-B755-4CC2-983C-F2D7C359B6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37100" yWindow="-4190" windowWidth="34980" windowHeight="18110" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="192">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -517,6 +517,9 @@
     <t>When player is caught by café worker enemy, player loses, game is paused, and given option to restart level.</t>
   </si>
   <si>
+    <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected.</t>
+  </si>
+  <si>
     <t>Create staionery object that upon overlap causes player to start of level.</t>
   </si>
   <si>
@@ -538,6 +541,9 @@
     <t>May need to adjust bounce strength and z vector if bounce is too strong or too weak</t>
   </si>
   <si>
+    <t>Currently set as timer function for slowed movement speed period, will adjust to an on begin and end overlap.</t>
+  </si>
+  <si>
     <t>Currently set as a teleport back to start without losing items, can adjust cause player to lose game with a pause game and add UI for chance to restart</t>
   </si>
   <si>
@@ -608,42 +614,6 @@
   </si>
   <si>
     <t>Need background added to the level map</t>
-  </si>
-  <si>
-    <t>Currently goes back to start point. Will setup respawn point actor blueprint soon.</t>
-  </si>
-  <si>
-    <t>Hairball movement was adjusted to a begin and end overlap for slowing player down.</t>
-  </si>
-  <si>
-    <t>Player takes damage on EventAnyDamage using float variables health, newHealth, and maxHealth, where health - damage clamped (0-maxHealth) sets health which sets newHealth, where if newHealth is &lt;= 0 then the game quits, if the player still has health a print string shows the players remaining health upon damage.</t>
-  </si>
-  <si>
-    <t>DamageTrap (Litter Box)</t>
-  </si>
-  <si>
-    <t>Created by casting to player and using apply damage node.</t>
-  </si>
-  <si>
-    <t>Create stationery object that when player comes into contact with will be unable to jkump and will sink into until reset back to start or spawn point</t>
-  </si>
-  <si>
-    <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected. ***Need to do respawn point logic</t>
-  </si>
-  <si>
-    <t>Has a begin and end overlap event incase player is able to escape. Set gravity to zero and pull character through the floor using velocity and setting new bool variable added to player called canJump? that gets set to false upon overlap with a current delay of 2 seconds before respawning back to start. ***Need to do respawn point logic</t>
-  </si>
-  <si>
-    <t>Currentlt have set to restore health by 10 with the health clamped between 0-maxHealth (which is set to 100). Adds 10 health on overlap only if player has less than maxHealth. Disappears upon overlap regardless if pllayer is at full health or not.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Currently set to send back to start. Will setup respawn actor blueprint soon. </t>
-  </si>
-  <si>
-    <t>Currently set with a 5 second timer, can make speed boost longer</t>
-  </si>
-  <si>
-    <t>Had to put some of the logic into the player character blueprint because the destroy actor in actor blueprint was casuing issues with the set timer by event node.</t>
   </si>
 </sst>
 </file>
@@ -1017,60 +987,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1397,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1416,62 +1386,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
@@ -1555,29 +1525,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="19" t="s">
+    <row r="8" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>192</v>
-      </c>
+      <c r="H8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" ht="50.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1605,8 +1573,8 @@
       <c r="H10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="27" t="s">
-        <v>162</v>
+      <c r="I10" s="43" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
@@ -1632,7 +1600,7 @@
         <v>21</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
@@ -1655,10 +1623,10 @@
         <v>57</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
@@ -1701,57 +1669,53 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="19" t="s">
+    <row r="16" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="19" t="s">
+      <c r="H16" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>201</v>
-      </c>
+      <c r="H17" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="20" t="s">
@@ -1804,51 +1768,48 @@
         <v>21</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21"/>
-      <c r="B21" s="18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="B21" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="D21" s="18" t="s">
+      <c r="C21" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="H21" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="20"/>
+    </row>
+    <row r="22" spans="1:9" ht="151" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="19" t="s">
-        <v>193</v>
+        <v>51</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>20</v>
@@ -1857,15 +1818,15 @@
         <v>21</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="151" customHeight="1" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>52</v>
+        <v>160</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>18</v>
@@ -1874,7 +1835,7 @@
         <v>19</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>20</v>
@@ -1883,68 +1844,62 @@
         <v>21</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="D24" s="18" t="s">
+    </row>
+    <row r="25" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E26" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F26" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="G26" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="27" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="21" t="s">
-        <v>54</v>
-      </c>
       <c r="B27" s="21" t="s">
-        <v>55</v>
+        <v>175</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>56</v>
+        <v>176</v>
       </c>
       <c r="D27" s="21" t="s">
         <v>18</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="21" t="s">
-        <v>57</v>
-      </c>
       <c r="H27" s="21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="21" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D28" s="21" t="s">
         <v>18</v>
@@ -1961,10 +1916,10 @@
     </row>
     <row r="29" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="21" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D29" s="21" t="s">
         <v>18</v>
@@ -1979,36 +1934,42 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="21" customFormat="1" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="D30" s="21" t="s">
+    <row r="30" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="H30" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="18" t="s">
-        <v>143</v>
-      </c>
+      <c r="E31" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>18</v>
@@ -2026,114 +1987,114 @@
         <v>21</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="19" t="s">
+      <c r="E33" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H33" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I33" s="19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H33" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" s="44"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B34" s="20" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>18</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="D34" s="20"/>
       <c r="E34" s="20" t="s">
         <v>27</v>
       </c>
       <c r="F34" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G34" s="20" t="s">
-        <v>20</v>
-      </c>
+      <c r="G34" s="20"/>
       <c r="H34" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I34" s="28"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B35" s="20" t="s">
+      <c r="I34" s="44"/>
+    </row>
+    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B35" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="H35" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="I35" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="28"/>
-    </row>
-    <row r="36" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="B36" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="D36" s="18" t="s">
+    </row>
+    <row r="37" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A37" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E37" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="H36" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="I36" s="29" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A38" s="18" t="s">
-        <v>148</v>
-      </c>
+      <c r="F37" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B38" s="19" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>18</v>
@@ -2155,37 +2116,34 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B39" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="D39" s="19" t="s">
+      <c r="B39" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G39" s="19" t="s">
+      <c r="E39" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H39" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="I39" s="19" t="s">
-        <v>155</v>
+      <c r="H39" s="20" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B40" s="20" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>18</v>
@@ -2200,29 +2158,6 @@
         <v>20</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B41" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" s="20" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2245,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2261,26 +2196,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
@@ -2311,7 +2246,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -2325,12 +2260,12 @@
         <v>68</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2358,7 +2293,7 @@
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
       <c r="F7" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -2374,7 +2309,7 @@
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.35">
@@ -2388,11 +2323,11 @@
         <v>61</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2403,14 +2338,14 @@
         <v>78</v>
       </c>
       <c r="C10" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>181</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>179</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2421,12 +2356,12 @@
         <v>80</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
       <c r="F11" s="19" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2449,12 +2384,12 @@
         <v>84</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2465,44 +2400,40 @@
         <v>86</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="105.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19" t="s">
-        <v>191</v>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2518,52 +2449,44 @@
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18" t="s">
-        <v>199</v>
-      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
@@ -2578,48 +2501,40 @@
       <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C22" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="s">
-        <v>200</v>
-      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
@@ -2773,62 +2688,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" spans="1:9" s="24" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -2953,7 +2868,7 @@
         <v>134</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -2961,7 +2876,7 @@
         <v>135</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -2969,7 +2884,7 @@
         <v>136</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -2977,7 +2892,7 @@
         <v>137</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -2985,7 +2900,7 @@
         <v>138</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -2993,7 +2908,7 @@
         <v>139</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -3001,7 +2916,7 @@
         <v>140</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated README and Traceability Matrix files
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\BBanuelos_GAM305\TeamRepo\GAM-305-Unreal-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spise\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F578C5E-2266-4115-81B6-C1517955C23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A65C83-9024-4BFA-9AA1-A48A32D4D853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="870" windowWidth="19420" windowHeight="10300" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="220">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -701,12 +701,6 @@
   </si>
   <si>
     <t>Kitten Sprites</t>
-  </si>
-  <si>
-    <t>ALexis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changed to a different enemy type. Customer enemy no longer exists. </t>
   </si>
 </sst>
 </file>
@@ -834,21 +828,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF8B1500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -918,13 +911,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1040,31 +1028,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1144,6 +1116,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1153,6 +1128,57 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1186,72 +1212,16 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="11" xfId="5" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -1576,81 +1546,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="24.53125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="23.46484375" style="10" customWidth="1"/>
     <col min="3" max="3" width="40" style="10" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" style="10" customWidth="1"/>
-    <col min="5" max="8" width="23.453125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="60.81640625" style="10" customWidth="1"/>
-    <col min="10" max="12" width="23.453125" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="8.81640625" style="10"/>
+    <col min="4" max="4" width="25.53125" style="10" customWidth="1"/>
+    <col min="5" max="8" width="23.46484375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="60.796875" style="10" customWidth="1"/>
+    <col min="10" max="12" width="23.46484375" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="8.796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-    </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
-    </row>
-    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="36"/>
+    </row>
+    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="52"/>
-    </row>
-    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40"/>
+    </row>
+    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="55"/>
-    </row>
-    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
+    </row>
+    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
@@ -1677,7 +1647,7 @@
       </c>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
         <v>14</v>
       </c>
@@ -1706,7 +1676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="19" t="s">
         <v>22</v>
       </c>
@@ -1732,7 +1702,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="19" t="s">
         <v>25</v>
       </c>
@@ -1756,8 +1726,8 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="50.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="50.55" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="1:9" ht="50.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="18" t="s">
         <v>28</v>
       </c>
@@ -1786,7 +1756,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="19" t="s">
         <v>31</v>
       </c>
@@ -1812,7 +1782,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="18" t="s">
         <v>33</v>
       </c>
@@ -1838,7 +1808,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -1848,8 +1818,8 @@
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="55.05" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="1:9" ht="81.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
         <v>35</v>
       </c>
@@ -1878,7 +1848,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="19" t="s">
         <v>39</v>
       </c>
@@ -1904,7 +1874,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="59.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="19" t="s">
         <v>41</v>
       </c>
@@ -1930,7 +1900,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="50.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="19" t="s">
         <v>43</v>
       </c>
@@ -1956,8 +1926,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="s">
         <v>45</v>
       </c>
@@ -1986,7 +1956,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21"/>
       <c r="B21" s="18" t="s">
         <v>48</v>
@@ -2013,7 +1983,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B22" s="19" t="s">
         <v>180</v>
       </c>
@@ -2039,7 +2009,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="151" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="151.05000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="19" t="s">
         <v>50</v>
       </c>
@@ -2065,7 +2035,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="64.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="18" t="s">
         <v>52</v>
       </c>
@@ -2091,35 +2061,34 @@
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:9" s="21" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="18.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="H27" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="19"/>
-    </row>
-    <row r="28" spans="1:9" s="21" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H27" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28"/>
       <c r="B28" s="19" t="s">
         <v>160</v>
@@ -2144,7 +2113,7 @@
       </c>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" s="21" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29"/>
       <c r="B29" s="19" t="s">
         <v>162</v>
@@ -2169,60 +2138,56 @@
       </c>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" s="21" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30"/>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H30" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I30" s="19"/>
-    </row>
-    <row r="31" spans="1:9" s="31" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H30" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="32" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31"/>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G31" s="18" t="s">
+      <c r="G31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H31" s="18" t="s">
+      <c r="H31" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="I31" s="18" t="s">
+      <c r="I31" s="33" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="33" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="18" t="s">
         <v>133</v>
       </c>
@@ -2251,7 +2216,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="19" t="s">
         <v>135</v>
       </c>
@@ -2277,7 +2242,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B35" s="20" t="s">
         <v>158</v>
       </c>
@@ -2301,55 +2266,53 @@
       </c>
       <c r="I35" s="28"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B36" s="19" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B36" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19" t="s">
+      <c r="D36" s="20"/>
+      <c r="E36" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="H36" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" s="62"/>
-    </row>
-    <row r="37" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="B37" s="19" t="s">
+      <c r="G36" s="20"/>
+      <c r="H36" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I36" s="28"/>
+    </row>
+    <row r="37" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B37" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G37" s="19" t="s">
+      <c r="G37" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="H37" s="19" t="s">
+      <c r="H37" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="I37" s="63" t="s">
+      <c r="I37" s="29" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A39" s="18" t="s">
         <v>138</v>
       </c>
@@ -2378,7 +2341,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B40" s="19" t="s">
         <v>143</v>
       </c>
@@ -2404,57 +2367,53 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="64" t="s">
+    <row r="41" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B41" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="C41" s="64" t="s">
+      <c r="C41" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="D41" s="64" t="s">
+      <c r="D41" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E41" s="64" t="s">
+      <c r="E41" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="64" t="s">
+      <c r="F41" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G41" s="64" t="s">
+      <c r="G41" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H41" s="64" t="s">
+      <c r="H41" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I41" s="64" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="44" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="19" t="s">
+    </row>
+    <row r="42" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B42" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="E42" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F42" s="19" t="s">
+      <c r="F42" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G42" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H42" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I42" s="19"/>
-    </row>
-    <row r="44" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="G42" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" s="20" t="s">
         <v>196</v>
       </c>
@@ -2478,7 +2437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B45" s="20" t="s">
         <v>198</v>
       </c>
@@ -2499,7 +2458,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B46" s="20" t="s">
         <v>199</v>
       </c>
@@ -2520,7 +2479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B47" s="20" t="s">
         <v>200</v>
       </c>
@@ -2541,7 +2500,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B48" s="20" t="s">
         <v>201</v>
       </c>
@@ -2581,44 +2540,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.453125" customWidth="1"/>
-    <col min="2" max="2" width="35.54296875" customWidth="1"/>
+    <col min="1" max="1" width="30.46484375" customWidth="1"/>
+    <col min="2" max="2" width="35.53125" customWidth="1"/>
     <col min="3" max="3" width="23" style="26" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="35.453125" customWidth="1"/>
-    <col min="6" max="6" width="42.54296875" customWidth="1"/>
-    <col min="7" max="7" width="38.81640625" customWidth="1"/>
+    <col min="5" max="5" width="35.46484375" customWidth="1"/>
+    <col min="6" max="6" width="42.53125" customWidth="1"/>
+    <col min="7" max="7" width="38.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="58"/>
-    </row>
-    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="46"/>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="61"/>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="49"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>58</v>
       </c>
@@ -2639,28 +2598,28 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D5" s="19"/>
@@ -2669,56 +2628,54 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-    </row>
-    <row r="7" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="54"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="74.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="74.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
         <v>74</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="59" t="s">
         <v>60</v>
       </c>
       <c r="D9" s="20" t="s">
@@ -2729,14 +2686,14 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>76</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="59" t="s">
         <v>168</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -2747,14 +2704,14 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
         <v>78</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D11" s="19"/>
@@ -2763,54 +2720,54 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
         <v>80</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="36"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" s="45" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="43" t="s">
+    <row r="13" spans="1:7" s="63" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="61" t="s">
         <v>215</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="61" t="s">
         <v>217</v>
       </c>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-    </row>
-    <row r="14" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+    </row>
+    <row r="14" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
         <v>214</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="54"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="19" t="s">
         <v>82</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D15" s="19"/>
@@ -2819,14 +2776,14 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="19" t="s">
         <v>84</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D16" s="19"/>
@@ -2835,14 +2792,14 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="105.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
         <v>86</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="60" t="s">
         <v>60</v>
       </c>
       <c r="D17" s="18"/>
@@ -2851,14 +2808,14 @@
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="75.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="19" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D18" s="19"/>
@@ -2867,14 +2824,14 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="18" t="s">
         <v>90</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="60" t="s">
         <v>60</v>
       </c>
       <c r="D19" s="18"/>
@@ -2883,14 +2840,14 @@
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="s">
         <v>92</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="60" t="s">
         <v>60</v>
       </c>
       <c r="D20" s="18"/>
@@ -2899,56 +2856,54 @@
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="19" t="s">
         <v>94</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
     </row>
-    <row r="22" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="19" t="s">
         <v>96</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
     </row>
-    <row r="23" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19" t="s">
+    <row r="23" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="54"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" ht="73.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="19" t="s">
         <v>100</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D24" s="19" t="s">
@@ -2959,28 +2914,28 @@
         <v>191</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="19" t="s">
         <v>102</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="19" t="s">
         <v>104</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D26" s="19"/>
@@ -2989,14 +2944,14 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="18" t="s">
         <v>106</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="60" t="s">
         <v>60</v>
       </c>
       <c r="D27" s="18"/>
@@ -3005,14 +2960,14 @@
         <v>189</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="19" t="s">
         <v>108</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D28" s="19" t="s">
@@ -3023,100 +2978,100 @@
         <v>191</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="5"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="5"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="5"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="5"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="5"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="5"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="5"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="5"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="5"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="5"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="5"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="5"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="5"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="5"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="5"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="5"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="5"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="5"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="5"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="5"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="5"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="5"/>
       <c r="F53" s="3"/>
     </row>
@@ -3136,79 +3091,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AA2BE-4F3F-4DB7-8D45-0977C97C1494}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.1796875" style="36" customWidth="1"/>
-    <col min="2" max="2" width="38.6328125" style="26" customWidth="1"/>
-    <col min="3" max="3" width="28.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.19921875" style="54" customWidth="1"/>
+    <col min="2" max="2" width="38.59765625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="28.46484375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="9" width="17.1796875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="1"/>
+    <col min="5" max="9" width="17.19921875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-    </row>
-    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="33" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
-    </row>
-    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="36"/>
+    </row>
+    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="52"/>
-    </row>
-    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="35" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40"/>
+    </row>
+    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="55"/>
-    </row>
-    <row r="5" spans="1:9" s="24" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
+    </row>
+    <row r="5" spans="1:9" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A5" s="22" t="s">
         <v>110</v>
       </c>
@@ -3223,191 +3178,191 @@
       <c r="H5" s="22"/>
       <c r="I5" s="23"/>
     </row>
-    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
+    <row r="6" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="54" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="36" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="54" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="54" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="54" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="36" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="54" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="29" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:9" s="30" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="50" t="s">
         <v>219</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="50" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="32" t="s">
+    <row r="14" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="31" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
+    <row r="15" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="31" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="32" t="s">
+    <row r="17" spans="1:2" s="30" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A17" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="50" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="37" t="s">
+    <row r="19" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="56" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="32" t="s">
+    <row r="20" spans="1:2" s="30" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A20" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="50" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="37" t="s">
+    <row r="21" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="56" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="32" t="s">
+    <row r="23" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="31" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="32" t="s">
+    <row r="24" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="31" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="32" t="s">
+    <row r="25" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="31" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="37" t="s">
+    <row r="27" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="56" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="28" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="37" t="s">
+    <row r="28" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="56" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="37" t="s">
+    <row r="29" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="56" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="37" t="s">
+    <row r="30" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="56" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="37" t="s">
+    <row r="31" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="56" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="32" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="37" t="s">
+    <row r="32" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="56" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="37" t="s">
+    <row r="33" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="56" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="37" t="s">
+    <row r="34" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="55" t="s">
         <v>211</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="56" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="37" t="s">
+    <row r="36" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="56" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="37" t="s">
+    <row r="37" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="56" t="s">
         <v>208</v>
       </c>
     </row>
@@ -3435,18 +3390,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f716dd8a-49a0-4c40-b209-038e1651b548" xsi:nil="true"/>
-    <Notes xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003FC679AA94041F4BA4494D199A3447AF" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f196c085cfdbd30e0a6b7617037a918">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xmlns:ns3="f716dd8a-49a0-4c40-b209-038e1651b548" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c32ca31bb9a34b5b0e8feded347fb44b" ns2:_="" ns3:_="">
     <xsd:import namespace="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
@@ -3703,6 +3646,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f716dd8a-49a0-4c40-b209-038e1651b548" xsi:nil="true"/>
+    <Notes xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
   <ds:schemaRefs>
@@ -3712,17 +3667,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
-    <ds:schemaRef ds:uri="f716dd8a-49a0-4c40-b209-038e1651b548"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B87576-EBB2-43B7-B881-33A6175934F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3739,4 +3683,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
+    <ds:schemaRef ds:uri="f716dd8a-49a0-4c40-b209-038e1651b548"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Traceability Matrix and README
Brought the traceability matrix and read me file from the final-beta onto main
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spise\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A65C83-9024-4BFA-9AA1-A48A32D4D853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6345B1B-6586-4283-8861-9B75155F53E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="223">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Set player camera to fixed position thaat does not rotate with the player. Make so player is only able to move left or right.</t>
   </si>
   <si>
-    <t>Unreal Engine 5.7.1</t>
-  </si>
-  <si>
     <t>alpha</t>
   </si>
   <si>
@@ -644,12 +641,6 @@
   </si>
   <si>
     <t>Sound (Lose)</t>
-  </si>
-  <si>
-    <t>Adobe Audition / Unreal Engine 5.7.1</t>
-  </si>
-  <si>
-    <t>post-beta</t>
   </si>
   <si>
     <t>Concept Art Finished.</t>
@@ -701,13 +692,31 @@
   </si>
   <si>
     <t>Kitten Sprites</t>
+  </si>
+  <si>
+    <t>final release</t>
+  </si>
+  <si>
+    <t>restarting the game</t>
+  </si>
+  <si>
+    <t>When the player loses, returns to the main menu, then replays the level again, the player should be able to play the level as normal</t>
+  </si>
+  <si>
+    <t>Unreal Engine 5.7.2</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>Adobe Audition / Unreal Engine 5.7.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -836,6 +845,19 @@
     <font>
       <sz val="11"/>
       <color rgb="FF8B1500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1036,7 +1058,7 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1131,6 +1153,46 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1180,45 +1242,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1544,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:I3"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1563,62 +1595,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36"/>
+      <c r="B2" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="40"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="54"/>
     </row>
     <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
     </row>
     <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
@@ -1658,154 +1690,154 @@
         <v>16</v>
       </c>
       <c r="D6" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="F6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="19" t="s">
+      <c r="H6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="I6" s="19" t="s">
         <v>20</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="D7" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="19" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="I8" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="50.55" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="10" spans="1:9" ht="50.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>30</v>
-      </c>
       <c r="D10" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>18</v>
-      </c>
       <c r="F10" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>32</v>
-      </c>
       <c r="D11" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>18</v>
-      </c>
       <c r="F11" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>34</v>
-      </c>
       <c r="D12" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="F12" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
@@ -1821,704 +1853,730 @@
     <row r="14" spans="1:9" ht="55.05" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="15" spans="1:9" ht="81.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="D15" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="D16" s="19" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="I16" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="59.55" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>42</v>
-      </c>
       <c r="D17" s="19" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="I17" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="50.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>44</v>
-      </c>
       <c r="D18" s="19" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="I18" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="20" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="C20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>47</v>
-      </c>
       <c r="D20" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="F20" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="19" t="s">
+      <c r="H20" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="I20" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21"/>
       <c r="B21" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B22" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="19" t="s">
         <v>180</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="151.05000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>51</v>
-      </c>
       <c r="D23" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="F23" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="19" t="s">
+      <c r="H23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="I23" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="64.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18.7" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="1:9" s="67" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D24" s="18" t="s">
+      <c r="B27" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="67" t="s">
+        <v>220</v>
+      </c>
+      <c r="E27" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="18" t="s">
+      <c r="F27" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="67" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="67" t="s">
         <v>26</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="18.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="27" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28"/>
       <c r="B28" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="C28" s="19" t="s">
-        <v>161</v>
-      </c>
       <c r="D28" s="19" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I28" s="19"/>
     </row>
     <row r="29" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29"/>
       <c r="B29" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="C29" s="19" t="s">
-        <v>163</v>
-      </c>
       <c r="D29" s="19" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I29" s="19"/>
     </row>
     <row r="30" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30"/>
       <c r="B30" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="C30" s="21" t="s">
-        <v>165</v>
-      </c>
       <c r="D30" s="21" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="E30" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30" s="21" t="s">
         <v>26</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="21" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="32" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31"/>
       <c r="B31" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="C31" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="D31" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="E31" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="I31" s="33" t="s">
         <v>194</v>
-      </c>
-      <c r="D31" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="I31" s="33" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="33" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>134</v>
-      </c>
       <c r="C33" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D33" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E33" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="F33" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" s="19" t="s">
+      <c r="H33" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H33" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="I33" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D34" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E34" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="F34" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" s="19" t="s">
+      <c r="H34" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H34" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="I34" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B35" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="C35" s="20" t="s">
-        <v>159</v>
-      </c>
       <c r="D35" s="20" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="E35" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>27</v>
       </c>
       <c r="I35" s="28"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B36" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>175</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>176</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I36" s="28"/>
     </row>
     <row r="37" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B37" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="D37" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="D37" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G37" s="18" t="s">
+      <c r="H37" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I37" s="29" t="s">
         <v>173</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="I37" s="29" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A39" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="C39" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C39" s="19" t="s">
-        <v>140</v>
-      </c>
       <c r="D39" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E39" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="F39" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F39" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" s="19" t="s">
+      <c r="H39" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H39" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="I39" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B40" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D40" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E40" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="F40" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F40" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" s="19" t="s">
+      <c r="H40" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H40" s="19" t="s">
-        <v>20</v>
-      </c>
       <c r="I40" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B41" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="E41" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H41" s="20" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B42" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="E42" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F42" s="20" t="s">
+    </row>
+    <row r="43" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B43" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G42" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H42" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A44" s="20" t="s">
+    </row>
+    <row r="45" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="B45" s="20" t="s">
         <v>196</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="F44" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B45" s="20" t="s">
-        <v>198</v>
       </c>
       <c r="C45" s="20"/>
       <c r="D45" s="20" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="G45" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H45" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B46" s="20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C46" s="20"/>
       <c r="D46" s="20" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H46" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B47" s="20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C47" s="20"/>
       <c r="D47" s="20" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="G47" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B48" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C48" s="20"/>
       <c r="D48" s="20" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B49" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="G49" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2528,6 +2586,7 @@
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B4:I4"/>
   </mergeCells>
+  <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{59B140CE-31A8-49FF-9CF4-576CBDA95646}"/>
   </hyperlinks>
@@ -2540,8 +2599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2556,57 +2615,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="46"/>
+      <c r="A1" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="60"/>
     </row>
     <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="63"/>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="58" t="s">
-        <v>153</v>
+      <c r="C4" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -2614,41 +2673,41 @@
     </row>
     <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="58" t="s">
-        <v>153</v>
+      <c r="C5" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="65" customFormat="1" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
     </row>
     <row r="7" spans="1:7" ht="74.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="58" t="s">
-        <v>153</v>
+      <c r="C7" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -2656,13 +2715,13 @@
     </row>
     <row r="8" spans="1:7" ht="74.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="58" t="s">
-        <v>153</v>
+      <c r="C8" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
@@ -2670,201 +2729,201 @@
     </row>
     <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>60</v>
+      <c r="C9" s="43" t="s">
+        <v>59</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="59" t="s">
-        <v>168</v>
+      <c r="C10" s="43" t="s">
+        <v>167</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="58" t="s">
-        <v>153</v>
+      <c r="C11" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
       <c r="F11" s="19" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="65" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" s="63" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="61" t="s">
-        <v>213</v>
-      </c>
-      <c r="B13" s="61" t="s">
-        <v>215</v>
-      </c>
-      <c r="C13" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="D13" s="61" t="s">
-        <v>217</v>
-      </c>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+    </row>
+    <row r="13" spans="1:7" s="47" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
     </row>
     <row r="14" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="C14" s="54"/>
+        <v>213</v>
+      </c>
+      <c r="C14" s="38"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="58" t="s">
-        <v>153</v>
+      <c r="C15" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
       <c r="F15" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="58" t="s">
-        <v>153</v>
+      <c r="C16" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
       <c r="F16" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="105.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="60" t="s">
-        <v>60</v>
+      <c r="C17" s="44" t="s">
+        <v>59</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="75.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="58" t="s">
-        <v>153</v>
+      <c r="C18" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="60" t="s">
-        <v>60</v>
+      <c r="C19" s="44" t="s">
+        <v>59</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="60" t="s">
-        <v>60</v>
+      <c r="C20" s="44" t="s">
+        <v>59</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="58" t="s">
-        <v>153</v>
+      <c r="C21" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
@@ -2872,13 +2931,13 @@
     </row>
     <row r="22" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="58" t="s">
-        <v>153</v>
+      <c r="C22" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
@@ -2886,43 +2945,43 @@
     </row>
     <row r="23" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="54"/>
+      <c r="C23" s="38"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="73.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="58" t="s">
-        <v>153</v>
+      <c r="C24" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="58" t="s">
-        <v>153</v>
+      <c r="C25" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
@@ -2930,52 +2989,52 @@
     </row>
     <row r="26" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="58" t="s">
-        <v>153</v>
+      <c r="C26" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
       <c r="F26" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C27" s="60" t="s">
-        <v>60</v>
+      <c r="C27" s="44" t="s">
+        <v>59</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C28" s="58" t="s">
-        <v>153</v>
+      <c r="C28" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3092,12 +3151,12 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.19921875" style="54" customWidth="1"/>
+    <col min="1" max="1" width="28.19921875" style="38" customWidth="1"/>
     <col min="2" max="2" width="38.59765625" style="26" customWidth="1"/>
     <col min="3" max="3" width="28.46484375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
@@ -3106,69 +3165,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36"/>
+      <c r="B2" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="40"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="54"/>
     </row>
     <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
     </row>
     <row r="5" spans="1:9" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A5" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>110</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>111</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
@@ -3179,191 +3238,191 @@
       <c r="I5" s="23"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="54" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="54" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="38" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="54" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="38" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="54" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="38" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="54" t="s">
+    <row r="12" spans="1:9" s="30" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="34" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="30" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="50" t="s">
+      <c r="B14" s="31" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="30" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A17" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="50" t="s">
+      <c r="B19" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="30" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A17" s="50" t="s">
+    </row>
+    <row r="20" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="B34" s="40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="B17" s="50" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="B19" s="56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="30" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A20" s="50" t="s">
-        <v>119</v>
-      </c>
-      <c r="B20" s="50" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="B21" s="56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="50" t="s">
-        <v>121</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="50" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="55" t="s">
-        <v>124</v>
-      </c>
-      <c r="B27" s="56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="55" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" s="56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="55" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" s="56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="55" t="s">
-        <v>128</v>
-      </c>
-      <c r="B31" s="56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="B32" s="56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" s="56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="55" t="s">
-        <v>211</v>
-      </c>
-      <c r="B34" s="56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="55" t="s">
+    </row>
+    <row r="37" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="B36" s="56" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="55" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" s="56" t="s">
-        <v>208</v>
+      <c r="B37" s="40" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3381,12 +3440,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f716dd8a-49a0-4c40-b209-038e1651b548" xsi:nil="true"/>
+    <Notes xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3647,21 +3709,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f716dd8a-49a0-4c40-b209-038e1651b548" xsi:nil="true"/>
-    <Notes xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
+    <ds:schemaRef ds:uri="f716dd8a-49a0-4c40-b209-038e1651b548"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3686,12 +3748,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
-    <ds:schemaRef ds:uri="f716dd8a-49a0-4c40-b209-038e1651b548"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sounds for Pickups and Obstacles
The sounds for the pickups and obstacles have been added to their blueprints and work on overlap.

Have added sounds for the enemies but have not attached them yet. Wanted to wait until the enemy blueprints were good to work on so as not to cause merge conflicts.

Thinking about adding some looping background ambience for the game. I'll share a listen of the track over the stream meeting.

Updated Traceability Matrix
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spise\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\BBanuelos_GAM305\TeamRepo\GAM-305-Unreal-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6345B1B-6586-4283-8861-9B75155F53E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAFDE8C-D46F-4AF9-8186-15C9962C5428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="-38510" yWindow="-6520" windowWidth="38620" windowHeight="21100" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="241">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -586,18 +586,12 @@
     <t>Create stationery object that when player comes into contact with will be unable to jkump and will sink into until reset back to start or spawn point</t>
   </si>
   <si>
-    <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected. ***Need to do respawn point logic</t>
-  </si>
-  <si>
     <t>Has a begin and end overlap event incase player is able to escape. Set gravity to zero and pull character through the floor using velocity and setting new bool variable added to player called canJump? that gets set to false upon overlap with a current delay of 2 seconds before respawning back to start. ***Need to do respawn point logic</t>
   </si>
   <si>
     <t>Currentlt have set to restore health by 10 with the health clamped between 0-maxHealth (which is set to 100). Adds 10 health on overlap only if player has less than maxHealth. Disappears upon overlap regardless if pllayer is at full health or not.</t>
   </si>
   <si>
-    <t xml:space="preserve">Currently set to send back to start. Will setup respawn actor blueprint soon. </t>
-  </si>
-  <si>
     <t>Currently set with a 5 second timer, can make speed boost longer</t>
   </si>
   <si>
@@ -632,9 +626,6 @@
   </si>
   <si>
     <t>Sound (Obstacles)</t>
-  </si>
-  <si>
-    <t>Sound (Enemies)</t>
   </si>
   <si>
     <t>Sound (Win)</t>
@@ -709,14 +700,161 @@
     <t>final</t>
   </si>
   <si>
-    <t>Adobe Audition / Unreal Engine 5.7.2</t>
+    <t>Health is located in the bottom center of the screen</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Error 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Blueprint Runtime Error: "Accessed None trying to read (real) property PlayerWidget in BP_PaperPlayerChar_C". Node: Set kitten Graph: EventGraph Function: Execute Ubergraph BP Paper Player Char Blueprint: BP_PaperPlayerChar | </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Error 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Blueprint Runtime Error: "Attempted to assign to None". Node: Set kitten Graph: EventGraph Function: Execute Ubergraph BP Paper Player Char Blueprint: BP_PaperPlayer_Char</t>
+    </r>
+  </si>
+  <si>
+    <t>Player gets sent back and is spawning at checkpoint or start if they haven't overlapped checkpoint yet but is having collision and movement errors that locks up the controls</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Old Comment:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Currently set to send back to start. Will setup respawn actor blueprint soon. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF8B1500"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">New Comment: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF8B1500"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Need to work with level designer to verfiy collision information for environment meshes. Unsure as to why the runtime errors reference the Set kitten node. Doesn't appear everytime the game runs in editor.</t>
+    </r>
+  </si>
+  <si>
+    <t>Emma/Bri</t>
+  </si>
+  <si>
+    <t>Running into player collision problems with environment assets. Player gets stuck on objects and can't move after respawn.</t>
+  </si>
+  <si>
+    <t>Changing enemy from a customer to a toy car.</t>
+  </si>
+  <si>
+    <t>Café worker enemy shoots players with projectile (water) and causes damage. If player loses all 3 life points then player is presented with UI where they can choose to restart the level, or quit and be brought back to the Main Menu.</t>
+  </si>
+  <si>
+    <t>Player does not need to return to Main Menu to restart the level. They can do so from the Win or Lose UI overlays. Or they can quit from the win or lose UI overlays that will take them back to the main menu where they can select to play again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sound (Enemies) </t>
+  </si>
+  <si>
+    <t>Give toy car enemy a vroom or toy car noise / give café worker sraying or spritsing sound for when employee is spraying with water</t>
+  </si>
+  <si>
+    <t>Yarn - boingy sound/bounce sound / Hairball - squishy / Catnip - purring sound / Litterbox - crunchy sand noise</t>
+  </si>
+  <si>
+    <t>uplifting horns sound to indicate success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">down-trodden horns sound for lose </t>
+  </si>
+  <si>
+    <t>Lure will have a bell sound / Speed will be a chewing sound / Health will be a slurping sound / Collectible will be a kitten mew</t>
+  </si>
+  <si>
+    <t>Adobe Audition / Unreal Engine 5.7</t>
+  </si>
+  <si>
+    <t>Unreal Engine 5.7</t>
+  </si>
+  <si>
+    <t>Sounds added under their own folder under the Bri folder and organized by the type of item they belong to. Used Play Sound at location node and selected the sound to use and grabbed the actors location for the location for when player overlaps.</t>
+  </si>
+  <si>
+    <t>Used Play Sound at location node and selected the sound to use and grabbed the actors location for the location for when player overlaps.</t>
+  </si>
+  <si>
+    <t>Went a different direction for the car wit ha cat toy noise to use for idle movement and a horn to use for on player hit/overlap when they cause damage. Have a spraying sound added for the enemy when they fire the projectile.</t>
+  </si>
+  <si>
+    <t>Have sound but not imported to Unreal yet. Want to make sure there are no merge conflicts with just adding the sound to the blueprints first.</t>
+  </si>
+  <si>
+    <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected. ***Need to do respawn point logic *** Nixed checkpoint because it was causing critical bug where player was getting stuck in objects</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -858,6 +996,39 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF8B1500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1137,7 +1308,6 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1193,6 +1363,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1240,16 +1421,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1578,81 +1749,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.53125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="23.46484375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" style="10" customWidth="1"/>
     <col min="3" max="3" width="40" style="10" customWidth="1"/>
-    <col min="4" max="4" width="25.53125" style="10" customWidth="1"/>
-    <col min="5" max="8" width="23.46484375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="60.796875" style="10" customWidth="1"/>
-    <col min="10" max="12" width="23.46484375" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="8.796875" style="10"/>
+    <col min="4" max="4" width="25.54296875" style="10" customWidth="1"/>
+    <col min="5" max="8" width="23.453125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="60.81640625" style="10" customWidth="1"/>
+    <col min="10" max="12" width="23.453125" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-    </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="48" t="s">
-        <v>209</v>
-      </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
-    </row>
-    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="52" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="54"/>
+    </row>
+    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="54"/>
-    </row>
-    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="58"/>
+    </row>
+    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="57"/>
-    </row>
-    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="61"/>
+    </row>
+    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
@@ -1679,7 +1850,7 @@
       </c>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>14</v>
       </c>
@@ -1690,7 +1861,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>17</v>
@@ -1708,7 +1879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="19" t="s">
         <v>21</v>
       </c>
@@ -1716,7 +1887,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>17</v>
@@ -1734,13 +1905,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>25</v>
@@ -1758,8 +1929,8 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="50.55" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="10" spans="1:9" ht="50.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="50.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
         <v>27</v>
       </c>
@@ -1770,7 +1941,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>17</v>
@@ -1788,7 +1959,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="19" t="s">
         <v>30</v>
       </c>
@@ -1796,7 +1967,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>17</v>
@@ -1814,7 +1985,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="18" t="s">
         <v>32</v>
       </c>
@@ -1822,7 +1993,7 @@
         <v>33</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>17</v>
@@ -1840,7 +2011,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -1850,8 +2021,8 @@
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" ht="55.05" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="15" spans="1:9" ht="81.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>34</v>
       </c>
@@ -1862,7 +2033,7 @@
         <v>36</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>17</v>
@@ -1880,7 +2051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="19" t="s">
         <v>38</v>
       </c>
@@ -1888,7 +2059,7 @@
         <v>39</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>25</v>
@@ -1903,10 +2074,10 @@
         <v>19</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="59.55" customHeight="1" x14ac:dyDescent="0.45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
         <v>40</v>
       </c>
@@ -1914,7 +2085,7 @@
         <v>41</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>25</v>
@@ -1929,10 +2100,10 @@
         <v>19</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="50.2" customHeight="1" x14ac:dyDescent="0.45">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="19" t="s">
         <v>42</v>
       </c>
@@ -1940,7 +2111,7 @@
         <v>43</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>25</v>
@@ -1955,11 +2126,11 @@
         <v>19</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="20" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.45">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>44</v>
       </c>
@@ -1970,7 +2141,7 @@
         <v>46</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>17</v>
@@ -1988,7 +2159,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21" s="18" t="s">
         <v>47</v>
@@ -1997,7 +2168,7 @@
         <v>181</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>25</v>
@@ -2012,10 +2183,10 @@
         <v>156</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="B22" s="19" t="s">
         <v>179</v>
       </c>
@@ -2023,7 +2194,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>25</v>
@@ -2041,7 +2212,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="151.05000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" ht="151" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="19" t="s">
         <v>49</v>
       </c>
@@ -2049,7 +2220,7 @@
         <v>50</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>17</v>
@@ -2067,7 +2238,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="64.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="18" t="s">
         <v>51</v>
       </c>
@@ -2075,7 +2246,7 @@
         <v>148</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>17</v>
@@ -2090,37 +2261,38 @@
         <v>156</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="18.7" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="27" spans="1:9" s="67" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="66" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:9" s="49" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="67" t="s">
-        <v>220</v>
-      </c>
-      <c r="E27" s="67" t="s">
+      <c r="D27" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="E27" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="67" t="s">
+      <c r="F27" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="67" t="s">
+      <c r="G27" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="H27" s="67" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H27" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="19"/>
+    </row>
+    <row r="28" spans="1:9" s="21" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28"/>
       <c r="B28" s="19" t="s">
         <v>159</v>
@@ -2129,7 +2301,7 @@
         <v>160</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E28" s="19" t="s">
         <v>25</v>
@@ -2145,7 +2317,7 @@
       </c>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" s="21" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29"/>
       <c r="B29" s="19" t="s">
         <v>161</v>
@@ -2154,7 +2326,7 @@
         <v>162</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E29" s="19" t="s">
         <v>25</v>
@@ -2170,59 +2342,60 @@
       </c>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" s="21" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" s="21" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30"/>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="D30" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="E30" s="21" t="s">
+      <c r="D30" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="E30" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="21" t="s">
+      <c r="G30" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="H30" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="32" customFormat="1" ht="72.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H30" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="19"/>
+    </row>
+    <row r="31" spans="1:9" s="31" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31"/>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="I31" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C31" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="D31" s="33" t="s">
-        <v>220</v>
-      </c>
-      <c r="E31" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="H31" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="I31" s="33" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="33" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
         <v>132</v>
       </c>
@@ -2233,7 +2406,7 @@
         <v>135</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>17</v>
@@ -2251,7 +2424,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="19" t="s">
         <v>134</v>
       </c>
@@ -2259,7 +2432,7 @@
         <v>136</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>17</v>
@@ -2277,51 +2450,55 @@
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B35" s="20" t="s">
+    <row r="35" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B35" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="D35" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="E35" s="20" t="s">
+      <c r="D35" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B36" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G35" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" s="28"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B36" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20" t="s">
+      <c r="F36" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F36" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I36" s="28"/>
-    </row>
-    <row r="37" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="G36" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I36" s="50"/>
+    </row>
+    <row r="37" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="18" t="s">
         <v>170</v>
       </c>
@@ -2329,7 +2506,7 @@
         <v>171</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>17</v>
@@ -2343,11 +2520,11 @@
       <c r="H37" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="I37" s="29" t="s">
+      <c r="I37" s="28" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
         <v>137</v>
       </c>
@@ -2358,7 +2535,7 @@
         <v>139</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>17</v>
@@ -2376,7 +2553,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B40" s="19" t="s">
         <v>142</v>
       </c>
@@ -2384,7 +2561,7 @@
         <v>140</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>17</v>
@@ -2402,7 +2579,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B41" s="20" t="s">
         <v>143</v>
       </c>
@@ -2410,7 +2587,7 @@
         <v>146</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="E41" s="20" t="s">
         <v>25</v>
@@ -2419,116 +2596,137 @@
         <v>25</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="H41" s="20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B42" s="20" t="s">
+      <c r="I41" s="20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="B42" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D42" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="E42" s="20" t="s">
+      <c r="D42" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="E42" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G42" s="20" t="s">
+      <c r="G42" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="B43" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" s="19" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A45" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="G45" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H42" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B43" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="G43" s="20" t="s">
+      <c r="H45" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I45" s="19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B46" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="G46" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H43" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="F45" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H45" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B46" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="G46" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H46" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H46" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I46" s="19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="B47" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="C47" s="20"/>
+        <v>228</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>229</v>
+      </c>
       <c r="D47" s="20" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>18</v>
@@ -2536,20 +2734,25 @@
       <c r="H47" s="20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="I47" s="20" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B48" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="C48" s="20"/>
+        <v>196</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>231</v>
+      </c>
       <c r="D48" s="20" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>18</v>
@@ -2557,26 +2760,34 @@
       <c r="H48" s="20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="I48" s="20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B49" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="C49" s="20"/>
+        <v>197</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>232</v>
+      </c>
       <c r="D49" s="20" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>18</v>
       </c>
       <c r="H49" s="20" t="s">
         <v>26</v>
+      </c>
+      <c r="I49" s="20" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2599,44 +2810,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.46484375" customWidth="1"/>
-    <col min="2" max="2" width="35.53125" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
     <col min="3" max="3" width="23" style="26" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="35.46484375" customWidth="1"/>
-    <col min="6" max="6" width="42.53125" customWidth="1"/>
-    <col min="7" max="7" width="38.796875" customWidth="1"/>
+    <col min="5" max="5" width="35.453125" customWidth="1"/>
+    <col min="6" max="6" width="42.54296875" customWidth="1"/>
+    <col min="7" max="7" width="38.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="60"/>
-    </row>
-    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="64"/>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="63"/>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="67"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>57</v>
       </c>
@@ -2657,28 +2868,28 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>65</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D5" s="19"/>
@@ -2687,54 +2898,58 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="65" customFormat="1" ht="136.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="64" t="s">
+    <row r="6" spans="1:7" s="48" customFormat="1" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-    </row>
-    <row r="7" spans="1:7" ht="74.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C6" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:7" ht="74.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>71</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>73</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="42" t="s">
         <v>59</v>
       </c>
       <c r="D9" s="20" t="s">
@@ -2745,14 +2960,14 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>75</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="42" t="s">
         <v>167</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -2763,14 +2978,14 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>77</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D11" s="19"/>
@@ -2779,54 +2994,54 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="65" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="64" t="s">
+    <row r="12" spans="1:7" s="48" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-    </row>
-    <row r="13" spans="1:7" s="47" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="45" t="s">
+      <c r="C12" s="33"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+    </row>
+    <row r="13" spans="1:7" s="46" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+    </row>
+    <row r="14" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="B13" s="45" t="s">
-        <v>212</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>167</v>
-      </c>
-      <c r="D13" s="45" t="s">
-        <v>214</v>
-      </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-    </row>
-    <row r="14" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C14" s="38"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>81</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D15" s="19"/>
@@ -2835,14 +3050,14 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>83</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D16" s="19"/>
@@ -2851,14 +3066,14 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="105.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>85</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="43" t="s">
         <v>59</v>
       </c>
       <c r="D17" s="18"/>
@@ -2867,14 +3082,14 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="75.7" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
         <v>87</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D18" s="19"/>
@@ -2883,14 +3098,14 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>89</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="43" t="s">
         <v>59</v>
       </c>
       <c r="D19" s="18"/>
@@ -2899,238 +3114,250 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:6" ht="194.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C20" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
         <v>93</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
     </row>
-    <row r="22" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
         <v>95</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
     </row>
-    <row r="23" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" spans="1:6" ht="73.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C23" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="19" t="s">
         <v>99</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="19" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>101</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>103</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
       <c r="F26" s="19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
         <v>105</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C27" s="44" t="s">
+      <c r="C27" s="43" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="19" t="s">
         <v>107</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="41" t="s">
         <v>152</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="30" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.45">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="51"/>
+      <c r="B29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+    </row>
+    <row r="30" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="F53" s="3"/>
     </row>
@@ -3150,79 +3377,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AA2BE-4F3F-4DB7-8D45-0977C97C1494}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.19921875" style="38" customWidth="1"/>
-    <col min="2" max="2" width="38.59765625" style="26" customWidth="1"/>
-    <col min="3" max="3" width="28.46484375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1796875" style="37" customWidth="1"/>
+    <col min="2" max="2" width="38.6328125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="9" width="17.19921875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.19921875" style="1"/>
+    <col min="5" max="9" width="17.1796875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-    </row>
-    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="35" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="48" t="s">
-        <v>209</v>
-      </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
-    </row>
-    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="36" t="s">
+      <c r="B2" s="52" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="54"/>
+    </row>
+    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="54"/>
-    </row>
-    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="37" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="58"/>
+    </row>
+    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="57"/>
-    </row>
-    <row r="5" spans="1:9" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="61"/>
+    </row>
+    <row r="5" spans="1:9" s="24" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>109</v>
       </c>
@@ -3237,192 +3464,192 @@
       <c r="H5" s="22"/>
       <c r="I5" s="23"/>
     </row>
-    <row r="6" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="38" t="s">
+    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="38" t="s">
+      <c r="B6" s="37" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="37" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="38" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="37" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="38" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="37" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="38" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="37" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="30" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="34" t="s">
+    <row r="12" spans="1:9" s="29" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="33" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="34" t="s">
+    <row r="19" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="30" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A17" s="34" t="s">
+    </row>
+    <row r="20" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="34" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="B27" s="40" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="B30" s="40" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="B31" s="40" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="B32" s="40" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="B33" s="40" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="39" t="s">
-        <v>208</v>
-      </c>
-      <c r="B34" s="40" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="B36" s="40" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="41" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="39" t="s">
+    </row>
+    <row r="37" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="B37" s="40" t="s">
-        <v>205</v>
+      <c r="B37" s="39" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Matrix to reflect name change
Updated the traceability matrix to reflect the game name change from "Cat Momma Cafe" to "Cat Mama Cafe"
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\BBanuelos_GAM305\TeamRepo\GAM-305-Unreal-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAFDE8C-D46F-4AF9-8186-15C9962C5428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD8D5E68-A995-4509-9667-B782CD369258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-6520" windowWidth="38620" windowHeight="21100" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="-34720" yWindow="-4920" windowWidth="19200" windowHeight="11170" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="242">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -848,6 +848,9 @@
   </si>
   <si>
     <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected. ***Need to do respawn point logic *** Nixed checkpoint because it was causing critical bug where player was getting stuck in objects</t>
+  </si>
+  <si>
+    <t>Cat Mama Café</t>
   </si>
 </sst>
 </file>
@@ -1749,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1783,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>206</v>
+        <v>241</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
@@ -3679,6 +3682,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003FC679AA94041F4BA4494D199A3447AF" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f196c085cfdbd30e0a6b7617037a918">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xmlns:ns3="f716dd8a-49a0-4c40-b209-038e1651b548" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c32ca31bb9a34b5b0e8feded347fb44b" ns2:_="" ns3:_="">
     <xsd:import namespace="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
@@ -3935,15 +3947,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
   <ds:schemaRefs>
@@ -3956,6 +3959,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B87576-EBB2-43B7-B881-33A6175934F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3972,12 +3983,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Damage Indicator Fix 2
</commit_message>
<xml_diff>
--- a/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
+++ b/GAM_305_BlueTeam_TraceabilityMatrix_and_TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\BBanuelos_GAM305\TeamRepo\GAM-305-Unreal-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmak\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD8D5E68-A995-4509-9667-B782CD369258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830D8DB5-3803-4D73-81F6-01557918A078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34720" yWindow="-4920" windowWidth="19200" windowHeight="11170" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19EF330C-6F54-4365-A47E-10806019DE9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="242">
   <si>
     <t>Traceability Matrix</t>
   </si>
@@ -382,12 +382,6 @@
     <t>Player Jumping Animation</t>
   </si>
   <si>
-    <t>Player Hurt Animation</t>
-  </si>
-  <si>
-    <t>Player Death Animation</t>
-  </si>
-  <si>
     <t>Enemy Worker Roaming Sprite</t>
   </si>
   <si>
@@ -433,9 +427,6 @@
     <t>Floor Sprite</t>
   </si>
   <si>
-    <t>Parallax Background Sprite</t>
-  </si>
-  <si>
     <t>Level</t>
   </si>
   <si>
@@ -640,29 +631,15 @@
     <t>Car Toy Movement Animation</t>
   </si>
   <si>
-    <t>Enemy Worker Spraying VFX</t>
-  </si>
-  <si>
-    <t>Concept Art Finished.
-Sprite Finished.
-Waiting to be put in-game.</t>
-  </si>
-  <si>
     <t>Completed and in-game.</t>
   </si>
   <si>
     <t>Completed and In-Game.</t>
   </si>
   <si>
-    <t>Set up In-Game. WIP.</t>
-  </si>
-  <si>
     <t>Shelf</t>
   </si>
   <si>
-    <t>Cat Momma Café</t>
-  </si>
-  <si>
     <t>Player collides with car toy</t>
   </si>
   <si>
@@ -678,10 +655,6 @@
     <t>Car toy moves past the player without colliding.</t>
   </si>
   <si>
-    <t>Concept Art Finished.
-Waiting to be put in-game.</t>
-  </si>
-  <si>
     <t>Kitten Sprites</t>
   </si>
   <si>
@@ -701,13 +674,91 @@
   </si>
   <si>
     <t>Health is located in the bottom center of the screen</t>
+  </si>
+  <si>
+    <t>Player gets sent back and is spawning at checkpoint or start if they haven't overlapped checkpoint yet but is having collision and movement errors that locks up the controls</t>
+  </si>
+  <si>
+    <t>Emma/Bri</t>
+  </si>
+  <si>
+    <t>Running into player collision problems with environment assets. Player gets stuck on objects and can't move after respawn.</t>
+  </si>
+  <si>
+    <t>Changing enemy from a customer to a toy car.</t>
+  </si>
+  <si>
+    <t>Café worker enemy shoots players with projectile (water) and causes damage. If player loses all 3 life points then player is presented with UI where they can choose to restart the level, or quit and be brought back to the Main Menu.</t>
+  </si>
+  <si>
+    <t>Player does not need to return to Main Menu to restart the level. They can do so from the Win or Lose UI overlays. Or they can quit from the win or lose UI overlays that will take them back to the main menu where they can select to play again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sound (Enemies) </t>
+  </si>
+  <si>
+    <t>Give toy car enemy a vroom or toy car noise / give café worker sraying or spritsing sound for when employee is spraying with water</t>
+  </si>
+  <si>
+    <t>Yarn - boingy sound/bounce sound / Hairball - squishy / Catnip - purring sound / Litterbox - crunchy sand noise</t>
+  </si>
+  <si>
+    <t>uplifting horns sound to indicate success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">down-trodden horns sound for lose </t>
+  </si>
+  <si>
+    <t>Lure will have a bell sound / Speed will be a chewing sound / Health will be a slurping sound / Collectible will be a kitten mew</t>
+  </si>
+  <si>
+    <t>Adobe Audition / Unreal Engine 5.7</t>
+  </si>
+  <si>
+    <t>Unreal Engine 5.7</t>
+  </si>
+  <si>
+    <t>Sounds added under their own folder under the Bri folder and organized by the type of item they belong to. Used Play Sound at location node and selected the sound to use and grabbed the actors location for the location for when player overlaps.</t>
+  </si>
+  <si>
+    <t>Used Play Sound at location node and selected the sound to use and grabbed the actors location for the location for when player overlaps.</t>
+  </si>
+  <si>
+    <t>Went a different direction for the car wit ha cat toy noise to use for idle movement and a horn to use for on player hit/overlap when they cause damage. Have a spraying sound added for the enemy when they fire the projectile.</t>
+  </si>
+  <si>
+    <t>Have sound but not imported to Unreal yet. Want to make sure there are no merge conflicts with just adding the sound to the blueprints first.</t>
+  </si>
+  <si>
+    <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected. ***Need to do respawn point logic *** Nixed checkpoint because it was causing critical bug where player was getting stuck in objects</t>
+  </si>
+  <si>
+    <t>Cat Mama Café</t>
+  </si>
+  <si>
+    <t>Enemy Worker Spraying Sprite</t>
+  </si>
+  <si>
+    <t>Sprite Sheet Finished.</t>
+  </si>
+  <si>
+    <t>Sprite Finished.</t>
+  </si>
+  <si>
+    <t>Completed and In-Game</t>
+  </si>
+  <si>
+    <t>Background Sprite</t>
+  </si>
+  <si>
+    <t>Assets List</t>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF9C0006"/>
+        <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -717,7 +768,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF9C0006"/>
+        <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -728,7 +779,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF9C0006"/>
+        <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -738,7 +789,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF9C0006"/>
+        <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -747,15 +798,12 @@
     </r>
   </si>
   <si>
-    <t>Player gets sent back and is spawning at checkpoint or start if they haven't overlapped checkpoint yet but is having collision and movement errors that locks up the controls</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
         <i/>
         <sz val="11"/>
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -766,7 +814,7 @@
       <rPr>
         <i/>
         <sz val="11"/>
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -777,7 +825,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF8B1500"/>
+        <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -787,7 +835,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF8B1500"/>
+        <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -796,68 +844,17 @@
     </r>
   </si>
   <si>
-    <t>Emma/Bri</t>
-  </si>
-  <si>
-    <t>Running into player collision problems with environment assets. Player gets stuck on objects and can't move after respawn.</t>
-  </si>
-  <si>
-    <t>Changing enemy from a customer to a toy car.</t>
-  </si>
-  <si>
-    <t>Café worker enemy shoots players with projectile (water) and causes damage. If player loses all 3 life points then player is presented with UI where they can choose to restart the level, or quit and be brought back to the Main Menu.</t>
-  </si>
-  <si>
-    <t>Player does not need to return to Main Menu to restart the level. They can do so from the Win or Lose UI overlays. Or they can quit from the win or lose UI overlays that will take them back to the main menu where they can select to play again.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sound (Enemies) </t>
-  </si>
-  <si>
-    <t>Give toy car enemy a vroom or toy car noise / give café worker sraying or spritsing sound for when employee is spraying with water</t>
-  </si>
-  <si>
-    <t>Yarn - boingy sound/bounce sound / Hairball - squishy / Catnip - purring sound / Litterbox - crunchy sand noise</t>
-  </si>
-  <si>
-    <t>uplifting horns sound to indicate success</t>
-  </si>
-  <si>
-    <t xml:space="preserve">down-trodden horns sound for lose </t>
-  </si>
-  <si>
-    <t>Lure will have a bell sound / Speed will be a chewing sound / Health will be a slurping sound / Collectible will be a kitten mew</t>
-  </si>
-  <si>
-    <t>Adobe Audition / Unreal Engine 5.7</t>
-  </si>
-  <si>
-    <t>Unreal Engine 5.7</t>
-  </si>
-  <si>
-    <t>Sounds added under their own folder under the Bri folder and organized by the type of item they belong to. Used Play Sound at location node and selected the sound to use and grabbed the actors location for the location for when player overlaps.</t>
-  </si>
-  <si>
-    <t>Used Play Sound at location node and selected the sound to use and grabbed the actors location for the location for when player overlaps.</t>
-  </si>
-  <si>
-    <t>Went a different direction for the car wit ha cat toy noise to use for idle movement and a horn to use for on player hit/overlap when they cause damage. Have a spraying sound added for the enemy when they fire the projectile.</t>
-  </si>
-  <si>
-    <t>Have sound but not imported to Unreal yet. Want to make sure there are no merge conflicts with just adding the sound to the blueprints first.</t>
-  </si>
-  <si>
-    <t>Made as a teleport back to player start instead of full restart for player consideration, so they don't feel frustrated if they were almostto the goal but ran into some catnip. This way they don't lose the items they've collected. ***Need to do respawn point logic *** Nixed checkpoint because it was causing critical bug where player was getting stuck in objects</t>
-  </si>
-  <si>
-    <t>Cat Mama Café</t>
+    <t>Damage Indicator</t>
+  </si>
+  <si>
+    <t>Red tint appears on-screen when player receives damage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -978,20 +975,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF8B1500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="7"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1004,17 +987,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="7" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color theme="2" tint="-0.249977111117893"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1023,15 +1019,36 @@
       <b/>
       <i/>
       <sz val="11"/>
-      <color theme="2" tint="-0.249977111117893"/>
+      <color theme="5" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF8B1500"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1079,19 +1096,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF3CACE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1107,8 +1112,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1224,15 +1241,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1284,99 +1337,126 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1425,8 +1505,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent6" xfId="5" builtinId="50"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1437,6 +1521,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FF99"/>
       <color rgb="FF8B1500"/>
       <color rgb="FFF3CACE"/>
       <color rgb="FFAE2B00"/>
@@ -1750,83 +1835,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB4A1F4-D2AB-4474-B05F-C8B13F4E557C}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I2"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="10" customWidth="1"/>
     <col min="3" max="3" width="40" style="10" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" style="10" customWidth="1"/>
-    <col min="5" max="8" width="23.453125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="60.81640625" style="10" customWidth="1"/>
-    <col min="10" max="12" width="23.453125" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="8.81640625" style="10"/>
+    <col min="4" max="4" width="25.5703125" style="10" customWidth="1"/>
+    <col min="5" max="8" width="23.42578125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="60.85546875" style="10" customWidth="1"/>
+    <col min="10" max="12" width="23.42578125" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-    </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="52" t="s">
-        <v>241</v>
-      </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
-    </row>
-    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="63" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
+    </row>
+    <row r="3" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="58"/>
-    </row>
-    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="69"/>
+    </row>
+    <row r="4" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="61"/>
-    </row>
-    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
+    </row>
+    <row r="5" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
@@ -1853,142 +1938,144 @@
       </c>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:9" s="52" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="D6" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="40" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="1:9" s="51" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E7" s="19" t="s">
+      <c r="D7" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="40" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="19" t="s">
+    <row r="8" spans="1:9" s="51" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E8" s="19" t="s">
+      <c r="C8" s="40"/>
+      <c r="D8" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E8" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="19" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="50.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I8" s="40" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="50.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E10" s="19" t="s">
+      <c r="D10" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E10" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="19" t="s">
+      <c r="I10" s="53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E11" s="19" t="s">
+      <c r="D11" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="19" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I11" s="40" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>32</v>
       </c>
@@ -1996,7 +2083,7 @@
         <v>33</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>17</v>
@@ -2008,13 +2095,13 @@
         <v>55</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -2024,154 +2111,154 @@
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="55.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E15" s="19" t="s">
+      <c r="D15" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E15" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="19" t="s">
+    <row r="16" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E16" s="19" t="s">
+      <c r="D16" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E16" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="19" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="19" t="s">
+      <c r="I16" s="40" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E17" s="19" t="s">
+      <c r="D17" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="19" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="19" t="s">
+      <c r="I17" s="40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E18" s="19" t="s">
+      <c r="D18" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E18" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="40" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E20" s="19" t="s">
+      <c r="D20" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E20" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I20" s="40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>25</v>
@@ -2183,73 +2270,73 @@
         <v>18</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="B22" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C22" s="19" t="s">
+    </row>
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B22" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="C22" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E22" s="19" t="s">
+      <c r="D22" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E22" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="19" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="151" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="19" t="s">
+      <c r="I22" s="40" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="151.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E23" s="19" t="s">
+      <c r="D23" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E23" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="40" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
         <v>51</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>17</v>
@@ -2261,255 +2348,256 @@
         <v>18</v>
       </c>
       <c r="H24" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:9" s="37" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="27"/>
+    </row>
+    <row r="28" spans="1:9" s="38" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="B28" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="I24" s="18" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:9" s="49" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E27" s="19" t="s">
+      <c r="C28" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" s="27"/>
+    </row>
+    <row r="29" spans="1:9" s="38" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="B29" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" s="27"/>
+    </row>
+    <row r="30" spans="1:9" s="38" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+      <c r="B30" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="27"/>
+    </row>
+    <row r="31" spans="1:9" s="38" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="B31" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="H31" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" s="39" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="32.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E33" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F33" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" s="40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E34" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34" s="40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="54" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H27" s="19" t="s">
+      <c r="F35" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="G35" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="I35" s="42" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="H36" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I27" s="19"/>
-    </row>
-    <row r="28" spans="1:9" s="21" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28"/>
-      <c r="B28" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H28" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I28" s="19"/>
-    </row>
-    <row r="29" spans="1:9" s="21" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29"/>
-      <c r="B29" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H29" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I29" s="19"/>
-    </row>
-    <row r="30" spans="1:9" s="21" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30"/>
-      <c r="B30" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H30" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I30" s="19"/>
-    </row>
-    <row r="31" spans="1:9" s="31" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31"/>
-      <c r="B31" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>217</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="H31" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="I31" s="32" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I33" s="19" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H34" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I34" s="19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B35" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B36" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H36" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I36" s="50"/>
-    </row>
-    <row r="37" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="I36" s="41"/>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>17</v>
@@ -2518,279 +2606,302 @@
         <v>25</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="I37" s="28" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+      <c r="I37" s="20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E39" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B40" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D39" s="19" t="s">
+      <c r="D40" s="40" t="s">
+        <v>225</v>
+      </c>
+      <c r="E40" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B41" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="I41" s="31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B42" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>225</v>
+      </c>
+      <c r="E42" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H42" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="40" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B43" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="C43" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="D43" s="40" t="s">
+        <v>225</v>
+      </c>
+      <c r="E43" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="F43" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="G43" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" s="40" t="s">
         <v>217</v>
       </c>
-      <c r="E39" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="19" t="s">
+    </row>
+    <row r="45" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="C45" s="40" t="s">
+        <v>223</v>
+      </c>
+      <c r="D45" s="40" t="s">
+        <v>224</v>
+      </c>
+      <c r="E45" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="F45" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="G45" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H39" s="19" t="s">
+      <c r="H45" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="19" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B40" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" s="19" t="s">
+      <c r="I45" s="40" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B46" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="C46" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="D46" s="40" t="s">
+        <v>224</v>
+      </c>
+      <c r="E46" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="F46" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="G46" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H40" s="19" t="s">
+      <c r="H46" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="19" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B41" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G41" s="20" t="s">
+      <c r="I46" s="40" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B47" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="G47" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="I47" s="31" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B48" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="C48" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="D48" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="E48" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="F48" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="G48" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="I48" s="31" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B49" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="F49" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="G49" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="I49" s="31" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="79" t="s">
+        <v>240</v>
+      </c>
+      <c r="C50" s="79" t="s">
+        <v>241</v>
+      </c>
+      <c r="D50" s="79" t="s">
+        <v>225</v>
+      </c>
+      <c r="E50" s="79" t="s">
+        <v>206</v>
+      </c>
+      <c r="F50" s="79" t="s">
+        <v>206</v>
+      </c>
+      <c r="G50" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="H41" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I41" s="20" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="B42" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G42" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H42" s="19" t="s">
+      <c r="H50" s="79" t="s">
         <v>19</v>
-      </c>
-      <c r="I42" s="19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="B43" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="G43" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H43" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I43" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A45" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>234</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="G45" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H45" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I45" s="19" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B46" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>234</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="F46" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="G46" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H46" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I46" s="19" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="B47" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="G47" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H47" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I47" s="20" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B48" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="G48" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H48" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I48" s="20" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B49" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="F49" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="G49" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H49" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I49" s="20" t="s">
-        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2800,7 +2911,7 @@
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B4:I4"/>
   </mergeCells>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{59B140CE-31A8-49FF-9CF4-576CBDA95646}"/>
   </hyperlinks>
@@ -2813,44 +2924,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748CED0D-D7CE-4618-A56E-B7666AE2995E}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.453125" customWidth="1"/>
-    <col min="2" max="2" width="35.54296875" customWidth="1"/>
-    <col min="3" max="3" width="23" style="26" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23" style="19" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="35.453125" customWidth="1"/>
-    <col min="6" max="6" width="42.54296875" customWidth="1"/>
-    <col min="7" max="7" width="38.81640625" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="64"/>
-    </row>
-    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="75"/>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="67"/>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="78"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>57</v>
       </c>
@@ -2871,496 +2982,496 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:7" s="30" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+    </row>
+    <row r="5" spans="1:7" s="30" customFormat="1" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-    </row>
-    <row r="5" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="48" customFormat="1" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+    </row>
+    <row r="6" spans="1:7" s="30" customFormat="1" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
+      <c r="C6" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="30" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-    </row>
-    <row r="8" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+      <c r="C7" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+    </row>
+    <row r="8" spans="1:7" s="30" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-    </row>
-    <row r="9" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+      <c r="C8" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+    </row>
+    <row r="9" spans="1:7" s="33" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="33" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="30" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="48" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="47" t="s">
+    </row>
+    <row r="12" spans="1:7" s="26" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-    </row>
-    <row r="13" spans="1:7" s="46" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="44" t="s">
-        <v>207</v>
-      </c>
-      <c r="B13" s="44" t="s">
-        <v>209</v>
-      </c>
-      <c r="C13" s="45" t="s">
-        <v>167</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>211</v>
-      </c>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-    </row>
-    <row r="14" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="25"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+    </row>
+    <row r="13" spans="1:7" s="33" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+    </row>
+    <row r="14" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C14" s="37"/>
+        <v>203</v>
+      </c>
+      <c r="C14" s="21"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:7" s="44" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="19" t="s">
+      <c r="C15" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="44" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>85</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="22" t="s">
         <v>59</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="44" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>89</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="22" t="s">
         <v>59</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="194.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="33" customFormat="1" ht="194.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="42" t="s">
-        <v>167</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="19" t="s">
+      <c r="C20" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="44" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-    </row>
-    <row r="22" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="19" t="s">
+      <c r="C21" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+    </row>
+    <row r="22" spans="1:6" s="44" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-    </row>
-    <row r="23" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19" t="s">
+      <c r="C22" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+    </row>
+    <row r="23" spans="1:6" s="44" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
+      <c r="C23" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+    </row>
+    <row r="24" spans="1:6" s="44" customFormat="1" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="19" t="s">
+      <c r="C24" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="44" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-    </row>
-    <row r="26" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="19" t="s">
+      <c r="C25" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+    </row>
+    <row r="26" spans="1:6" s="44" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>105</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C27" s="22" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="44" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="51"/>
-      <c r="B29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-    </row>
-    <row r="30" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+    </row>
+    <row r="30" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="F53" s="3"/>
     </row>
@@ -3378,56 +3489,56 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AA2BE-4F3F-4DB7-8D45-0977C97C1494}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.1796875" style="37" customWidth="1"/>
-    <col min="2" max="2" width="38.6328125" style="26" customWidth="1"/>
-    <col min="3" max="3" width="28.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="9" width="17.1796875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="1"/>
+    <col min="5" max="9" width="17.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-    </row>
-    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>206</v>
-      </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
-    </row>
-    <row r="3" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="57" t="s">
-        <v>3</v>
+    <row r="1" spans="1:9" s="56" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+    </row>
+    <row r="2" spans="1:9" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+    </row>
+    <row r="3" spans="1:9" s="59" customFormat="1" ht="41.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>110</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
@@ -3435,241 +3546,214 @@
       <c r="F3" s="57"/>
       <c r="G3" s="57"/>
       <c r="H3" s="57"/>
-      <c r="I3" s="58"/>
-    </row>
-    <row r="4" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="61"/>
-    </row>
-    <row r="5" spans="1:9" s="24" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23"/>
-    </row>
-    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="37" t="s">
+      <c r="I3" s="57"/>
+    </row>
+    <row r="4" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="37" t="s">
+      <c r="B4" s="45" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="37" t="s">
+      <c r="B5" s="47" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
+      <c r="B6" s="45" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="37" t="s">
+      <c r="B10" s="47" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="45" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="48" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="29" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="33" t="s">
+      <c r="B15" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B16" s="50" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="33" t="s">
+    <row r="17" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="50" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="B17" s="33" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="B23" s="30" t="s">
+      <c r="B30" s="50" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="B30" s="39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="B31" s="39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="38" t="s">
+    <row r="32" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="B32" s="39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="B33" s="39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="38" t="s">
-        <v>205</v>
-      </c>
-      <c r="B34" s="39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="B36" s="39" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="B37" s="39" t="s">
-        <v>202</v>
+      <c r="B32" s="50" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="B33" s="50" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:I4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{3A43779C-E316-4C5A-BB83-78382714F424}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{FE22566E-E43A-41CC-9667-9038BDD65AB8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382">
@@ -3679,15 +3763,6 @@
     <Notes xmlns="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3948,20 +4023,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F271AB-EFB2-4823-A2F0-9F2289E658DB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="ff8a4b2e-b0c8-4039-a689-d1a7f36f4382"/>
     <ds:schemaRef ds:uri="f716dd8a-49a0-4c40-b209-038e1651b548"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8F3069D-89E7-4007-93BF-1DB2942FF756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>